<commit_message>
Update navigation fuel demand
Add low-energy demand (LED) scenario file
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_BASE.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_BASE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GDrive\PhD\TIMES-Ireland\Model-TIM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DC4808-802F-4277-A728-A3C69683973A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CED9C99-D783-4CD5-8060-E76A629B4BE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY-Demands" sheetId="4" r:id="rId1"/>
@@ -59,30 +59,19 @@
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -11024,107 +11013,107 @@
       </c>
       <c r="G59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.6676209897560728E-2</v>
+        <v>5.2718404005341231E-2</v>
       </c>
       <c r="H59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.86798323423325485</v>
+        <v>1.2476395718090483</v>
       </c>
       <c r="I59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1433394823130551</v>
+        <v>0.20603624964526884</v>
       </c>
       <c r="J59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.3926327207102271E-2</v>
+        <v>9.1887737410560347E-2</v>
       </c>
       <c r="K59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.4562723067759833E-2</v>
+        <v>7.8428487740469136E-2</v>
       </c>
       <c r="L59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.6330828482101425E-2</v>
+        <v>3.7847947145898793E-2</v>
       </c>
       <c r="M59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.3028466177847607E-2</v>
+        <v>0.11934516233092819</v>
       </c>
       <c r="N59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12564945344024189</v>
+        <v>0.18060859254580552</v>
       </c>
       <c r="O59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.0223319044188384E-2</v>
+        <v>7.2191026042654552E-2</v>
       </c>
       <c r="P59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.7186593701371281E-2</v>
+        <v>8.2200040812796776E-2</v>
       </c>
       <c r="Q59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.6452531059555369E-2</v>
+        <v>0.13864092047508828</v>
       </c>
       <c r="R59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.1751724770956333E-2</v>
+        <v>0.13188397896544515</v>
       </c>
       <c r="S59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.6543195942501155E-2</v>
+        <v>0.11002323137607375</v>
       </c>
       <c r="T59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.34972143460038307</v>
+        <v>0.50268977983509444</v>
       </c>
       <c r="U59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.515444627518814E-2</v>
+        <v>0.1367750527017661</v>
       </c>
       <c r="V59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12555604287263242</v>
+        <v>0.18047432414524395</v>
       </c>
       <c r="W59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10278576754348148</v>
+        <v>0.14774431803316554</v>
       </c>
       <c r="X59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.4841835190385328E-2</v>
+        <v>0.10757769450791341</v>
       </c>
       <c r="Y59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16624375349091422</v>
+        <v>0.23895886146297948</v>
       </c>
       <c r="Z59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.0643091230897193E-2</v>
+        <v>2.967239053514998E-2</v>
       </c>
       <c r="AA59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.4074020324263338E-2</v>
+        <v>0.12084804242824897</v>
       </c>
       <c r="AB59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1579942591656024E-2</v>
+        <v>5.9767032040341915E-2</v>
       </c>
       <c r="AC59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2218355505456412E-2</v>
+        <v>6.068468710900795E-2</v>
       </c>
       <c r="AD59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.9073402746374416E-2</v>
+        <v>7.0538135732292492E-2</v>
       </c>
       <c r="AE59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10255320744067464</v>
+        <v>0.1474100360152161</v>
       </c>
       <c r="AF59" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E59,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F59,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E59,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.9545524850201352E-2</v>
+        <v>5.6842758875006623E-2</v>
       </c>
     </row>
     <row r="60" spans="4:32" x14ac:dyDescent="0.2">
@@ -11140,107 +11129,107 @@
       </c>
       <c r="G60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.6775125500158448E-2</v>
+        <v>6.1129511486040324E-2</v>
       </c>
       <c r="H60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.87032418180931859</v>
+        <v>1.4466977704335002</v>
       </c>
       <c r="I60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14372606836730231</v>
+        <v>0.23890888821207609</v>
       </c>
       <c r="J60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.4098736275411433E-2</v>
+        <v>0.10654822742539792</v>
       </c>
       <c r="K60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.4709878530297934E-2</v>
+        <v>9.0941583544108057E-2</v>
       </c>
       <c r="L60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.6401842629241463E-2</v>
+        <v>4.3886505356722477E-2</v>
       </c>
       <c r="M60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.3252393644390243E-2</v>
+        <v>0.13838642518033492</v>
       </c>
       <c r="N60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12598832955197292</v>
+        <v>0.20942430334931633</v>
       </c>
       <c r="O60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.0358771150106334E-2</v>
+        <v>8.3708948306105369E-2</v>
       </c>
       <c r="P60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.734082573331465E-2</v>
+        <v>9.5314879762098764E-2</v>
       </c>
       <c r="Q60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.6712663179490302E-2</v>
+        <v>0.16076077985514226</v>
       </c>
       <c r="R60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.1999178833697487E-2</v>
+        <v>0.15292578292347522</v>
       </c>
       <c r="S60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.6749632659178113E-2</v>
+        <v>0.12757720027817143</v>
       </c>
       <c r="T60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.35066463201749509</v>
+        <v>0.58289284833492172</v>
       </c>
       <c r="U60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.5411077465255248E-2</v>
+        <v>0.15859721690909456</v>
       </c>
       <c r="V60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12589466705640764</v>
+        <v>0.20926861271548172</v>
       </c>
       <c r="W60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10306298037881616</v>
+        <v>0.17131660482913227</v>
       </c>
       <c r="X60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.5043683343399323E-2</v>
+        <v>0.12474148328536191</v>
       </c>
       <c r="Y60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16669211227991096</v>
+        <v>0.27708423162833901</v>
       </c>
       <c r="Z60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.0698765571683417E-2</v>
+        <v>3.4406556348954558E-2</v>
       </c>
       <c r="AA60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.4300767646476135E-2</v>
+        <v>0.14012908655077402</v>
       </c>
       <c r="AB60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1692083543213451E-2</v>
+        <v>6.9302732898106317E-2</v>
       </c>
       <c r="AC60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2332218254283814E-2</v>
+        <v>7.0366797850728177E-2</v>
       </c>
       <c r="AD60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.9205753532285394E-2</v>
+        <v>8.1792342917175062E-2</v>
       </c>
       <c r="AE60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10282979306227122</v>
+        <v>0.17092898883731</v>
       </c>
       <c r="AF60" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E60,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F60,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E60,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.9652178984625995E-2</v>
+        <v>6.5911898266037938E-2</v>
       </c>
     </row>
     <row r="61" spans="4:32" x14ac:dyDescent="0.2">
@@ -11256,107 +11245,107 @@
       </c>
       <c r="G61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.6795944695286409E-2</v>
+        <v>7.1311121771731364E-2</v>
       </c>
       <c r="H61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.87081689118064598</v>
+        <v>1.6876568839885906</v>
       </c>
       <c r="I61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14380743480784106</v>
+        <v>0.27870107915930081</v>
       </c>
       <c r="J61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.4135023958453261E-2</v>
+        <v>0.12429468902642533</v>
       </c>
       <c r="K61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.4740850977599148E-2</v>
+        <v>0.10608863346975926</v>
       </c>
       <c r="L61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.641678928424155E-2</v>
+        <v>5.1196154713974089E-2</v>
       </c>
       <c r="M61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.3299524627754112E-2</v>
+        <v>0.16143579390198537</v>
       </c>
       <c r="N61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12605965427435289</v>
+        <v>0.2443056002748121</v>
       </c>
       <c r="O61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.038728034127072E-2</v>
+        <v>9.7651344840264706E-2</v>
       </c>
       <c r="P61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.7373287616816183E-2</v>
+        <v>0.1111903372387515</v>
       </c>
       <c r="Q61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.6767414312999539E-2</v>
+        <v>0.18753677674958194</v>
       </c>
       <c r="R61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.2051261561620273E-2</v>
+        <v>0.17839679825649613</v>
       </c>
       <c r="S61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.6793082288692596E-2</v>
+        <v>0.14882620592200888</v>
       </c>
       <c r="T61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.35086315086139169</v>
+        <v>0.6799783259674046</v>
       </c>
       <c r="U61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.5465091742898162E-2</v>
+        <v>0.18501285504702344</v>
       </c>
       <c r="V61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12596593875442011</v>
+        <v>0.24412397811755615</v>
       </c>
       <c r="W61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10312132656444552</v>
+        <v>0.19985075901154031</v>
       </c>
       <c r="X61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.5086167198053749E-2</v>
+        <v>0.14551817752674534</v>
       </c>
       <c r="Y61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1667864802953738</v>
+        <v>0.32323483211848264</v>
       </c>
       <c r="Z61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.071048359122744E-2</v>
+        <v>4.0137244186983868E-2</v>
       </c>
       <c r="AA61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.4348492137071338E-2</v>
+        <v>0.16346870949665121</v>
       </c>
       <c r="AB61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1715686334795318E-2</v>
+        <v>8.0845658744372786E-2</v>
       </c>
       <c r="AC61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2356183439991521E-2</v>
+        <v>8.2086952246722744E-2</v>
       </c>
       <c r="AD61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.9233609975200932E-2</v>
+        <v>9.5415513456112752E-2</v>
       </c>
       <c r="AE61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10288800723550964</v>
+        <v>0.19939858246830361</v>
       </c>
       <c r="AF61" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E61,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F61,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E61,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.9674626942051074E-2</v>
+        <v>7.6890053415996307E-2</v>
       </c>
     </row>
     <row r="62" spans="4:32" x14ac:dyDescent="0.2">
@@ -11372,107 +11361,107 @@
       </c>
       <c r="G62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.6800315336518785E-2</v>
+        <v>8.2425010647798155E-2</v>
       </c>
       <c r="H62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.87092032725877799</v>
+        <v>1.9506794056314021</v>
       </c>
       <c r="I62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14382451632889723</v>
+        <v>0.32213683989983982</v>
       </c>
       <c r="J62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.4142641949579013E-2</v>
+        <v>0.1436661044158348</v>
       </c>
       <c r="K62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.4747353124027495E-2</v>
+        <v>0.12262262219554143</v>
       </c>
       <c r="L62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.6419927084056959E-2</v>
+        <v>5.9175111715861928E-2</v>
       </c>
       <c r="M62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.3309418988124259E-2</v>
+        <v>0.18659567681323028</v>
       </c>
       <c r="N62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1260746277049109</v>
+        <v>0.28238080125042475</v>
       </c>
       <c r="O62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.0393265368340157E-2</v>
+        <v>0.11287037615248005</v>
       </c>
       <c r="P62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.7380102445422201E-2</v>
+        <v>0.12851943011320616</v>
       </c>
       <c r="Q62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.6778908396232072E-2</v>
+        <v>0.21676451633896013</v>
       </c>
       <c r="R62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.2062195457803822E-2</v>
+        <v>0.2062000657189744</v>
       </c>
       <c r="S62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.6802203810495934E-2</v>
+        <v>0.17202087560843529</v>
       </c>
       <c r="T62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.35090482656687438</v>
+        <v>0.78595343006303864</v>
       </c>
       <c r="U62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.5476431135586098E-2</v>
+        <v>0.21384723965000949</v>
       </c>
       <c r="V62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12598090105340046</v>
+        <v>0.28217087315121997</v>
       </c>
       <c r="W62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10313357536864262</v>
+        <v>0.2309976414650477</v>
       </c>
       <c r="X62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.5095085971604872E-2</v>
+        <v>0.16819728864291794</v>
       </c>
       <c r="Y62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16680629127926941</v>
+        <v>0.37361120982487001</v>
       </c>
       <c r="Z62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.0712943593118299E-2</v>
+        <v>4.6392662144278278E-2</v>
       </c>
       <c r="AA62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.4358511094341643E-2</v>
+        <v>0.18894542374433004</v>
       </c>
       <c r="AB62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1720641345469496E-2</v>
+        <v>9.3445511966055772E-2</v>
       </c>
       <c r="AC62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2361214529241208E-2</v>
+        <v>9.4880261940621394E-2</v>
       </c>
       <c r="AD62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.9239457968711042E-2</v>
+        <v>0.11028608886226862</v>
       </c>
       <c r="AE62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10290022832591687</v>
+        <v>0.23047499288702816</v>
       </c>
       <c r="AF62" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E62,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F62,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E62,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.9679339514641018E-2</v>
+        <v>8.8873422743373481E-2</v>
       </c>
     </row>
     <row r="63" spans="4:32" x14ac:dyDescent="0.2">
@@ -11488,107 +11477,107 @@
       </c>
       <c r="G63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.6801232383767285E-2</v>
+        <v>9.3941042041646661E-2</v>
       </c>
       <c r="H63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.87094203020024663</v>
+        <v>2.2232190765156914</v>
       </c>
       <c r="I63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1438281003709295</v>
+        <v>0.36714427068141908</v>
       </c>
       <c r="J63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.4144240355265864E-2</v>
+        <v>0.16373845085148392</v>
       </c>
       <c r="K63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.4748717403357336E-2</v>
+        <v>0.13975487314342289</v>
       </c>
       <c r="L63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.642058545671536E-2</v>
+        <v>6.7442777548096342E-2</v>
       </c>
       <c r="M63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.3311495021244047E-2</v>
+        <v>0.21266593941009621</v>
       </c>
       <c r="N63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12607776942773</v>
+        <v>0.32183370694813068</v>
       </c>
       <c r="O63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.0394521145768326E-2</v>
+        <v>0.12864008955611639</v>
       </c>
       <c r="P63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.7381532331676852E-2</v>
+        <v>0.14647555508390686</v>
       </c>
       <c r="Q63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.6781320082948499E-2</v>
+        <v>0.24704982604790748</v>
       </c>
       <c r="R63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.2064489606162703E-2</v>
+        <v>0.23500936051397323</v>
       </c>
       <c r="S63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.6804117686750495E-2</v>
+        <v>0.19605481613613324</v>
       </c>
       <c r="T63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.35091357095677284</v>
+        <v>0.89576311408460396</v>
       </c>
       <c r="U63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.5478810365157082E-2</v>
+        <v>0.24372496130200105</v>
       </c>
       <c r="V63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12598404044059369</v>
+        <v>0.32159444869098125</v>
       </c>
       <c r="W63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10313614541079186</v>
+        <v>0.26327153588264596</v>
       </c>
       <c r="X63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.5096957307253395E-2</v>
+        <v>0.1916970157421195</v>
       </c>
       <c r="Y63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1668104480167607</v>
+        <v>0.42581039533449128</v>
       </c>
       <c r="Z63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.0713459750323928E-2</v>
+        <v>5.2874424773107102E-2</v>
       </c>
       <c r="AA63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.4360613270363219E-2</v>
+        <v>0.21534398183322534</v>
       </c>
       <c r="AB63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1721681005021376E-2</v>
+        <v>0.10650127551352571</v>
       </c>
       <c r="AC63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2362270151587708E-2</v>
+        <v>0.10813648194687206</v>
       </c>
       <c r="AD63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.9240684993779579E-2</v>
+        <v>0.12569473790775804</v>
       </c>
       <c r="AE63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10290279255316313</v>
+        <v>0.26267586532519177</v>
       </c>
       <c r="AF63" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E63,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F63,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E63,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.9680328305872613E-2</v>
+        <v>0.10129039567850284</v>
       </c>
     </row>
     <row r="64" spans="4:32" x14ac:dyDescent="0.2">
@@ -11604,107 +11593,107 @@
       </c>
       <c r="G64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.6801424764864192E-2</v>
+        <v>0.10621861626141103</v>
       </c>
       <c r="H64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.87094658311253403</v>
+        <v>2.5137815040286462</v>
       </c>
       <c r="I64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14382885224269906</v>
+        <v>0.41512799467134481</v>
       </c>
       <c r="J64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.4144575673909299E-2</v>
+        <v>0.18513816006555789</v>
       </c>
       <c r="K64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.4749003606226795E-2</v>
+        <v>0.15802006150306919</v>
       </c>
       <c r="L64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.6420723572231658E-2</v>
+        <v>7.6257175269666425E-2</v>
       </c>
       <c r="M64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.3311930538093867E-2</v>
+        <v>0.24046020055918832</v>
       </c>
       <c r="N64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12607842850836415</v>
+        <v>0.36389559105758984</v>
       </c>
       <c r="O64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.0394784586762768E-2</v>
+        <v>0.14545263722257901</v>
       </c>
       <c r="P64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.7381832297776263E-2</v>
+        <v>0.16561909937338348</v>
       </c>
       <c r="Q64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.6781826014280453E-2</v>
+        <v>0.2793378708615723</v>
       </c>
       <c r="R64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.2064970879923089E-2</v>
+        <v>0.26572378312779216</v>
       </c>
       <c r="S64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.6804519185815892E-2</v>
+        <v>0.22167809541790345</v>
       </c>
       <c r="T64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.35091540538277777</v>
+        <v>1.0128343949378156</v>
       </c>
       <c r="U64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.5479309487525518E-2</v>
+        <v>0.27557846469690617</v>
       </c>
       <c r="V64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12598469903125281</v>
+        <v>0.36362506307055448</v>
       </c>
       <c r="W64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10313668456243159</v>
+        <v>0.2976796683825767</v>
       </c>
       <c r="X64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.5097349882014761E-2</v>
+        <v>0.21675075463334667</v>
       </c>
       <c r="Y64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16681132003041041</v>
+        <v>0.48146145709244736</v>
       </c>
       <c r="Z64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.0713568031428917E-2</v>
+        <v>5.9784819424588347E-2</v>
       </c>
       <c r="AA64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.4361054271554353E-2</v>
+        <v>0.24348824830373031</v>
       </c>
       <c r="AB64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1721899108118375E-2</v>
+        <v>0.12042040272564668</v>
       </c>
       <c r="AC64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2362491603410685E-2</v>
+        <v>0.12226932158876516</v>
       </c>
       <c r="AD64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.9240942403012307E-2</v>
+        <v>0.14212234441665939</v>
       </c>
       <c r="AE64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10290333048493398</v>
+        <v>0.2970061469803722</v>
       </c>
       <c r="AF64" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E64,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F64,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E64,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.9680535737651124E-2</v>
+        <v>0.11452848973903919</v>
       </c>
     </row>
     <row r="65" spans="4:32" x14ac:dyDescent="0.2">
@@ -11720,107 +11709,107 @@
       </c>
       <c r="G65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.6801465127711944E-2</v>
+        <v>0.12002940589326376</v>
       </c>
       <c r="H65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.87094753834414684</v>
+        <v>2.8406291768239722</v>
       </c>
       <c r="I65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14382900999045209</v>
+        <v>0.46910389462648</v>
       </c>
       <c r="J65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.4144646026015453E-2</v>
+        <v>0.20921025092391538</v>
       </c>
       <c r="K65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.4749063653513313E-2</v>
+        <v>0.17856619459955325</v>
       </c>
       <c r="L65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.6420752549795701E-2</v>
+        <v>8.6172309194747512E-2</v>
       </c>
       <c r="M65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.3312021912457485E-2</v>
+        <v>0.2717253908021397</v>
       </c>
       <c r="N65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12607856678791302</v>
+        <v>0.41121013565386411</v>
       </c>
       <c r="O65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.0394839858454846E-2</v>
+        <v>0.16436472480932934</v>
       </c>
       <c r="P65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.7381895232680967E-2</v>
+        <v>0.18715327691184286</v>
       </c>
       <c r="Q65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.6781932162075909E-2</v>
+        <v>0.31565802552433248</v>
       </c>
       <c r="R65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.206507185439422E-2</v>
+        <v>0.30027380268299175</v>
       </c>
       <c r="S65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.6804603423019591E-2</v>
+        <v>0.25050119300252804</v>
       </c>
       <c r="T65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.35091579025768876</v>
+        <v>1.144525460522454</v>
       </c>
       <c r="U65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.5479414206754654E-2</v>
+        <v>0.31140981269367551</v>
       </c>
       <c r="V65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12598483720800163</v>
+        <v>0.41090443299359369</v>
       </c>
       <c r="W65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10313679768007102</v>
+        <v>0.3363846658906739</v>
       </c>
       <c r="X65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.5097432246839457E-2</v>
+        <v>0.24493318799718641</v>
       </c>
       <c r="Y65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16681150298473776</v>
+        <v>0.54406218692482022</v>
       </c>
       <c r="Z65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.0713590749532853E-2</v>
+        <v>6.7558179625584094E-2</v>
       </c>
       <c r="AA65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.4361146796569655E-2</v>
+        <v>0.27514715230296105</v>
       </c>
       <c r="AB65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1721944867614706E-2</v>
+        <v>0.13607774141036361</v>
       </c>
       <c r="AC65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2362538065492242E-2</v>
+        <v>0.13816706097124723</v>
       </c>
       <c r="AD65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.9240996409200218E-2</v>
+        <v>0.16060141964668845</v>
       </c>
       <c r="AE65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1029034433466367</v>
+        <v>0.33562357168131191</v>
       </c>
       <c r="AF65" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E65,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F65,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E65,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.9680579258233074E-2</v>
+        <v>0.12941974829909172</v>
       </c>
     </row>
     <row r="66" spans="4:32" x14ac:dyDescent="0.2">
@@ -11836,107 +11825,107 @@
       </c>
       <c r="G66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.68014736043882E-2</v>
+        <v>0.13651547417316809</v>
       </c>
       <c r="H66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.87094773895410349</v>
+        <v>3.2307902895820644</v>
       </c>
       <c r="I66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14382904311934927</v>
+        <v>0.53353542937937526</v>
       </c>
       <c r="J66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.4144660800791301E-2</v>
+        <v>0.23794533009821922</v>
       </c>
       <c r="K66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.4749076264154949E-2</v>
+        <v>0.20309230513673895</v>
       </c>
       <c r="L66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.6420758635427487E-2</v>
+        <v>9.8008096955664536E-2</v>
       </c>
       <c r="M66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.3312041102156467E-2</v>
+        <v>0.30904693974099989</v>
       </c>
       <c r="N66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1260785958282567</v>
+        <v>0.46768994844079709</v>
       </c>
       <c r="O66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.0394851466165062E-2</v>
+        <v>0.18694025999463149</v>
       </c>
       <c r="P66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.738190844975663E-2</v>
+        <v>0.21285882530654368</v>
       </c>
       <c r="Q66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.6781954454370628E-2</v>
+        <v>0.35901373259599417</v>
       </c>
       <c r="R66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.2065093060229544E-2</v>
+        <v>0.34151648298168796</v>
       </c>
       <c r="S66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.6804621113830449E-2</v>
+        <v>0.28490759317841136</v>
       </c>
       <c r="T66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.35091587108598021</v>
+        <v>1.3017263126789758</v>
       </c>
       <c r="U66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.5479436199033513E-2</v>
+        <v>0.35418202669318077</v>
       </c>
       <c r="V66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12598486622675606</v>
+        <v>0.46734225744530944</v>
       </c>
       <c r="W66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10313682143611555</v>
+        <v>0.38258718209006204</v>
       </c>
       <c r="X66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.5097449544428541E-2</v>
+        <v>0.27857482132266531</v>
       </c>
       <c r="Y66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16681154140731422</v>
+        <v>0.61878926147297497</v>
       </c>
       <c r="Z66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.0713595520603853E-2</v>
+        <v>7.6837312133861607E-2</v>
       </c>
       <c r="AA66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.4361166227919143E-2</v>
+        <v>0.31293868102152833</v>
       </c>
       <c r="AB66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1721954477651112E-2</v>
+        <v>0.15476805250180856</v>
       </c>
       <c r="AC66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2362547823079862E-2</v>
+        <v>0.15714434061579741</v>
       </c>
       <c r="AD66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.9241007751139557E-2</v>
+        <v>0.18266006394673046</v>
       </c>
       <c r="AE66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10290346704893148</v>
+        <v>0.38172155140474556</v>
       </c>
       <c r="AF66" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E66,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F66,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E66,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.968058839807094E-2</v>
+        <v>0.14719558240697844</v>
       </c>
     </row>
     <row r="67" spans="4:32" x14ac:dyDescent="0.2">
@@ -11952,107 +11941,107 @@
       </c>
       <c r="G67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.6801475373849528E-2</v>
+        <v>0.15648937130390672</v>
       </c>
       <c r="H67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.87094778083037083</v>
+        <v>3.7034947451461573</v>
       </c>
       <c r="I67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14382905003483135</v>
+        <v>0.61159824128090468</v>
       </c>
       <c r="J67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.4144663884947606E-2</v>
+        <v>0.27275966579830807</v>
       </c>
       <c r="K67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.474907889655968E-2</v>
+        <v>0.23280721354118941</v>
       </c>
       <c r="L67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.6420759905770929E-2</v>
+        <v>0.11234788999691867</v>
       </c>
       <c r="M67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.3312045107904645E-2</v>
+        <v>0.35426431762686589</v>
       </c>
       <c r="N67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12607860189027481</v>
+        <v>0.53611875459494229</v>
       </c>
       <c r="O67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.0394853889213172E-2</v>
+        <v>0.21429192503730549</v>
       </c>
       <c r="P67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.7381911208751267E-2</v>
+        <v>0.24400269603470487</v>
       </c>
       <c r="Q67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.6781959107769239E-2</v>
+        <v>0.41154186837566925</v>
       </c>
       <c r="R67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.2065097486835501E-2</v>
+        <v>0.39148455539870214</v>
       </c>
       <c r="S67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.680462480669363E-2</v>
+        <v>0.32659308701988854</v>
       </c>
       <c r="T67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.35091588795845852</v>
+        <v>1.4921849227325457</v>
       </c>
       <c r="U67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.54794407898054E-2</v>
+        <v>0.40600322432351199</v>
       </c>
       <c r="V67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12598487228426755</v>
+        <v>0.53572019211972532</v>
       </c>
       <c r="W67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1031368263950642</v>
+        <v>0.43856440419539355</v>
       </c>
       <c r="X67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.5097453155208757E-2</v>
+        <v>0.31933375255748392</v>
       </c>
       <c r="Y67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16681154942782381</v>
+        <v>0.70932576020416582</v>
       </c>
       <c r="Z67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.0713596516539687E-2</v>
+        <v>8.8079558316279061E-2</v>
       </c>
       <c r="AA67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.4361170284110568E-2</v>
+        <v>0.35872546864257293</v>
       </c>
       <c r="AB67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1721956483695387E-2</v>
+        <v>0.17741252689944778</v>
       </c>
       <c r="AC67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2362549859924672E-2</v>
+        <v>0.18013649526455311</v>
       </c>
       <c r="AD67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.9241010118709405E-2</v>
+        <v>0.20938548353204536</v>
       </c>
       <c r="AE67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10290347199666017</v>
+        <v>0.43757212106744053</v>
       </c>
       <c r="AF67" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E67,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F67,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E67,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.9680590305963749E-2</v>
+        <v>0.16873211105988936</v>
       </c>
     </row>
     <row r="68" spans="4:32" x14ac:dyDescent="0.2">
@@ -12068,107 +12057,107 @@
       </c>
       <c r="G68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.680147574447995E-2</v>
+        <v>0.15879131806522273</v>
       </c>
       <c r="H68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.87094778960175101</v>
+        <v>3.7579728714438461</v>
       </c>
       <c r="I68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14382905148334446</v>
+        <v>0.62059480493895047</v>
       </c>
       <c r="J68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.4144664530953327E-2</v>
+        <v>0.27677193975704673</v>
       </c>
       <c r="K68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.4749079447941752E-2</v>
+        <v>0.23623178996294136</v>
       </c>
       <c r="L68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.6420760171856381E-2</v>
+        <v>0.11400051892222025</v>
       </c>
       <c r="M68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.3312045946946467E-2</v>
+        <v>0.35947551882101775</v>
       </c>
       <c r="N68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12607860316002184</v>
+        <v>0.54400502073901114</v>
       </c>
       <c r="O68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.0394854396743516E-2</v>
+        <v>0.21744414297201631</v>
       </c>
       <c r="P68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.7381911786648795E-2</v>
+        <v>0.24759195715326776</v>
       </c>
       <c r="Q68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.6781960082467602E-2</v>
+        <v>0.41759561798920392</v>
       </c>
       <c r="R68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.2065098414029989E-2</v>
+        <v>0.39724326346236466</v>
       </c>
       <c r="S68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.6804625580198765E-2</v>
+        <v>0.33139724651436059</v>
       </c>
       <c r="T68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.3509158914925587</v>
+        <v>1.514134849564944</v>
       </c>
       <c r="U68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.5479441751385993E-2</v>
+        <v>0.41197550090388341</v>
       </c>
       <c r="V68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12598487355307061</v>
+        <v>0.54360059544006767</v>
       </c>
       <c r="W68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10313682743376289</v>
+        <v>0.44501565325757741</v>
       </c>
       <c r="X68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.5097453911520839E-2</v>
+        <v>0.3240311277936016</v>
       </c>
       <c r="Y68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16681155110779541</v>
+        <v>0.71975988823992232</v>
       </c>
       <c r="Z68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.0713596725147866E-2</v>
+        <v>8.9375201926544134E-2</v>
       </c>
       <c r="AA68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.436117113371823E-2</v>
+        <v>0.36400229302919329</v>
       </c>
       <c r="AB68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1721956903880329E-2</v>
+        <v>0.18002225168976571</v>
       </c>
       <c r="AC68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2362550286561079E-2</v>
+        <v>0.18278628942254588</v>
       </c>
       <c r="AD68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.9241010614619309E-2</v>
+        <v>0.212465528085021</v>
       </c>
       <c r="AE68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10290347303300873</v>
+        <v>0.44400877372020908</v>
       </c>
       <c r="AF68" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E68,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F68,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E68,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.9680590705589942E-2</v>
+        <v>0.17121414759277323</v>
       </c>
     </row>
     <row r="69" spans="4:32" x14ac:dyDescent="0.2">
@@ -12184,107 +12173,107 @@
       </c>
       <c r="G69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.6801475828170692E-2</v>
+        <v>0.1710449267488203</v>
       </c>
       <c r="H69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.87094779158238533</v>
+        <v>4.0479681279309414</v>
       </c>
       <c r="I69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14382905181042807</v>
+        <v>0.66848486582799671</v>
       </c>
       <c r="J69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.4144664676825586E-2</v>
+        <v>0.29812987724195417</v>
       </c>
       <c r="K69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.474907957244738E-2</v>
+        <v>0.25446132510441999</v>
       </c>
       <c r="L69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.6420760231940194E-2</v>
+        <v>0.12279771114671054</v>
       </c>
       <c r="M69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.3312046136407553E-2</v>
+        <v>0.38721552622593569</v>
       </c>
       <c r="N69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12607860344673893</v>
+        <v>0.58598480103978401</v>
       </c>
       <c r="O69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.0394854511347148E-2</v>
+        <v>0.23422387294078517</v>
       </c>
       <c r="P69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.738191191714178E-2</v>
+        <v>0.26669813369445644</v>
       </c>
       <c r="Q69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.6781960302560768E-2</v>
+        <v>0.44982063729865379</v>
       </c>
       <c r="R69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.2065098623396499E-2</v>
+        <v>0.4278977322454986</v>
       </c>
       <c r="S69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.6804625754861203E-2</v>
+        <v>0.35697050975751049</v>
       </c>
       <c r="T69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.35091589229058134</v>
+        <v>1.6309776100308899</v>
       </c>
       <c r="U69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.5479441968517098E-2</v>
+        <v>0.44376682700920456</v>
       </c>
       <c r="V69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12598487383957455</v>
+        <v>0.58554916704873206</v>
       </c>
       <c r="W69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10313682766830776</v>
+        <v>0.47935662189198391</v>
       </c>
       <c r="X69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.5097454082300993E-2</v>
+        <v>0.34903596237565787</v>
       </c>
       <c r="Y69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16681155148714383</v>
+        <v>0.77530232043397518</v>
       </c>
       <c r="Z69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.0713596772252943E-2</v>
+        <v>9.6272107650165306E-2</v>
       </c>
       <c r="AA69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.4361171325565129E-2</v>
+        <v>0.3920916225533671</v>
       </c>
       <c r="AB69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1721956998760801E-2</v>
+        <v>0.19391420909288029</v>
       </c>
       <c r="AC69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2362550382898344E-2</v>
+        <v>0.1968915420937952</v>
       </c>
       <c r="AD69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.924101072659897E-2</v>
+        <v>0.22886106829231614</v>
       </c>
       <c r="AE69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10290347326702294</v>
+        <v>0.47827204347288349</v>
       </c>
       <c r="AF69" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E69,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F69,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E69,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.9680590795828113E-2</v>
+        <v>0.18442640120500042</v>
       </c>
     </row>
     <row r="70" spans="4:32" x14ac:dyDescent="0.2">
@@ -16890,8 +16879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CL75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R48" sqref="R48"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21636,250 +21625,250 @@
         <v>3.5132998087277101</v>
       </c>
       <c r="I22">
-        <v>3.063821683</v>
+        <v>4.2966351471015702</v>
       </c>
       <c r="J22">
-        <v>3.0676449140000002</v>
+        <v>4.4094344637268001</v>
       </c>
       <c r="K22">
-        <v>3.070448576</v>
+        <v>4.5291674028165003</v>
       </c>
       <c r="L22">
-        <v>3.0725033769999999</v>
+        <v>4.6611834502685596</v>
       </c>
       <c r="M22">
-        <v>3.0740086999999998</v>
+        <v>4.8042664418927696</v>
       </c>
       <c r="N22">
-        <v>3.0751111400000002</v>
+        <v>4.9555896582088499</v>
       </c>
       <c r="O22">
-        <v>3.0759183409999999</v>
+        <v>5.1129502074838999</v>
       </c>
       <c r="P22">
-        <v>3.0765092699999999</v>
+        <v>5.2752039056523996</v>
       </c>
       <c r="Q22">
-        <v>3.07694182</v>
+        <v>5.4414060135777298</v>
       </c>
       <c r="R22">
-        <v>3.0772584119999999</v>
+        <v>5.6117259844700902</v>
       </c>
       <c r="S22">
-        <v>3.0774901159999999</v>
+        <v>5.7862882839617802</v>
       </c>
       <c r="T22">
-        <v>3.077659685</v>
+        <v>5.9645530611175701</v>
       </c>
       <c r="U22">
-        <v>3.0777837770000001</v>
+        <v>6.1457480291828999</v>
       </c>
       <c r="V22">
-        <v>3.0778745870000002</v>
+        <v>6.3299271732513001</v>
       </c>
       <c r="W22">
-        <v>3.0779410390000002</v>
+        <v>6.5164111808959202</v>
       </c>
       <c r="X22">
-        <v>3.0779896670000002</v>
+        <v>6.7046092152599002</v>
       </c>
       <c r="Y22">
-        <v>3.0780252510000001</v>
+        <v>6.8941328835870399</v>
       </c>
       <c r="Z22">
-        <v>3.0780512889999998</v>
+        <v>7.0848817136199704</v>
       </c>
       <c r="AA22">
-        <v>3.0780703429999998</v>
+        <v>7.2761374036976303</v>
       </c>
       <c r="AB22">
-        <v>3.0780842860000002</v>
+        <v>7.4682763498887699</v>
       </c>
       <c r="AC22">
-        <v>3.0780944880000001</v>
+        <v>7.6618204080974204</v>
       </c>
       <c r="AD22">
-        <v>3.0781019540000001</v>
+        <v>7.8573484184930402</v>
       </c>
       <c r="AE22">
-        <v>3.0781074159999999</v>
+        <v>8.0554527175184294</v>
       </c>
       <c r="AF22">
-        <v>3.0781114139999999</v>
+        <v>8.2566896515540797</v>
       </c>
       <c r="AG22">
-        <v>3.0781143389999999</v>
+        <v>8.4615630814728604</v>
       </c>
       <c r="AH22">
-        <v>3.0781164790000002</v>
+        <v>8.6705693702179794</v>
       </c>
       <c r="AI22">
-        <v>3.0781180450000001</v>
+        <v>8.8842603654121408</v>
       </c>
       <c r="AJ22">
-        <v>3.0781191919999999</v>
+        <v>9.1033168790680801</v>
       </c>
       <c r="AK22">
-        <v>3.07812003</v>
+        <v>9.3273565167733494</v>
       </c>
       <c r="AL22">
-        <v>3.0781206440000002</v>
+        <v>9.5573045230475095</v>
       </c>
       <c r="AM22">
-        <v>3.078121093</v>
+        <v>9.7942615939640305</v>
       </c>
       <c r="AN22">
-        <v>3.0781214210000001</v>
+        <v>10.039412402408599</v>
       </c>
       <c r="AO22">
-        <v>3.078121662</v>
+        <v>10.293860643626401</v>
       </c>
       <c r="AP22">
-        <v>3.0781218379999999</v>
+        <v>10.5584100956768</v>
       </c>
       <c r="AQ22">
-        <v>3.078121967</v>
+        <v>10.833663592103999</v>
       </c>
       <c r="AR22">
-        <v>3.0781220610000002</v>
+        <v>11.1201369904683</v>
       </c>
       <c r="AS22">
-        <v>3.0781221300000001</v>
+        <v>11.4183281532989</v>
       </c>
       <c r="AT22">
-        <v>3.0781221799999998</v>
+        <v>11.7286584642425</v>
       </c>
       <c r="AU22">
-        <v>3.0781222170000002</v>
+        <v>12.051195404665901</v>
       </c>
       <c r="AV22">
-        <v>3.0781222439999998</v>
+        <v>12.3857005404062</v>
       </c>
       <c r="AW22">
-        <v>3.0781222640000001</v>
+        <v>12.7317569865743</v>
       </c>
       <c r="AX22">
-        <v>3.0781222779999999</v>
+        <v>13.088970352070501</v>
       </c>
       <c r="AY22">
-        <v>3.078122289</v>
+        <v>12.461582160250099</v>
       </c>
       <c r="AZ22">
-        <v>3.0781222970000002</v>
+        <v>12.666563648039499</v>
       </c>
       <c r="BA22">
-        <v>3.0781223020000001</v>
+        <v>12.871545135828899</v>
       </c>
       <c r="BB22">
-        <v>3.078122306</v>
+        <v>13.0765266236182</v>
       </c>
       <c r="BC22">
-        <v>3.0781223089999998</v>
+        <v>13.281508111407501</v>
       </c>
       <c r="BD22">
-        <v>3.0781223120000001</v>
+        <v>13.486489599196901</v>
       </c>
       <c r="BE22">
-        <v>3.0781223130000002</v>
+        <v>13.6914710869862</v>
       </c>
       <c r="BF22">
-        <v>3.0781223139999998</v>
+        <v>13.8964525747756</v>
       </c>
       <c r="BG22">
-        <v>3.0781223149999999</v>
+        <v>14.101434062565</v>
       </c>
       <c r="BH22">
-        <v>3.078122316</v>
+        <v>14.3064155503543</v>
       </c>
       <c r="BI22">
-        <v>3.078122316</v>
+        <v>14.511397038143601</v>
       </c>
       <c r="BJ22">
-        <v>3.0781223170000001</v>
+        <v>14.716378525933001</v>
       </c>
       <c r="BK22">
-        <v>3.0781223170000001</v>
+        <v>14.921360013722399</v>
       </c>
       <c r="BL22">
-        <v>3.0781223170000001</v>
+        <v>15.1263415015117</v>
       </c>
       <c r="BM22">
-        <v>3.0781223170000001</v>
+        <v>15.3313229893011</v>
       </c>
       <c r="BN22">
-        <v>3.0781223170000001</v>
+        <v>15.5363044770905</v>
       </c>
       <c r="BO22">
-        <v>3.0781223170000001</v>
+        <v>15.7412859648798</v>
       </c>
       <c r="BP22">
-        <v>3.0781223180000001</v>
+        <v>15.946267452669099</v>
       </c>
       <c r="BQ22">
-        <v>3.0781223180000001</v>
+        <v>16.151248940458501</v>
       </c>
       <c r="BR22">
-        <v>3.0781223180000001</v>
+        <v>16.356230428247802</v>
       </c>
       <c r="BS22">
-        <v>3.0781223180000001</v>
+        <v>16.561211916037202</v>
       </c>
       <c r="BT22">
-        <v>3.0781223180000001</v>
+        <v>16.766193403826598</v>
       </c>
       <c r="BU22">
-        <v>3.0781223180000001</v>
+        <v>16.971174891615899</v>
       </c>
       <c r="BV22">
-        <v>3.0781223180000001</v>
+        <v>17.176156379405199</v>
       </c>
       <c r="BW22">
-        <v>3.0781223180000001</v>
+        <v>17.3811378671946</v>
       </c>
       <c r="BX22">
-        <v>3.0781223180000001</v>
+        <v>17.586119354984</v>
       </c>
       <c r="BY22">
-        <v>3.0781223180000001</v>
+        <v>17.7911008427733</v>
       </c>
       <c r="BZ22">
-        <v>3.0781223180000001</v>
+        <v>17.9960823305627</v>
       </c>
       <c r="CA22">
-        <v>3.0781223180000001</v>
+        <v>18.201063818352001</v>
       </c>
       <c r="CB22">
-        <v>3.0781223180000001</v>
+        <v>18.406045306141401</v>
       </c>
       <c r="CC22">
-        <v>3.0781223180000001</v>
+        <v>18.611026793930701</v>
       </c>
       <c r="CD22">
-        <v>3.0781223180000001</v>
+        <v>18.816008281720102</v>
       </c>
       <c r="CE22">
-        <v>3.0781223180000001</v>
+        <v>19.020989769509399</v>
       </c>
       <c r="CF22">
-        <v>3.0781223180000001</v>
+        <v>19.225971257298799</v>
       </c>
       <c r="CG22">
-        <v>3.0781223180000001</v>
+        <v>19.430952745088199</v>
       </c>
       <c r="CH22">
-        <v>3.0781223180000001</v>
+        <v>19.635934232877499</v>
       </c>
       <c r="CI22">
-        <v>3.0781223180000001</v>
+        <v>19.8409157206668</v>
       </c>
       <c r="CJ22">
-        <v>3.0781223180000001</v>
+        <v>20.0458972084562</v>
       </c>
       <c r="CK22">
-        <v>3.0781223180000001</v>
+        <v>20.2508786962456</v>
       </c>
       <c r="CL22">
-        <v>3.0781223180000001</v>
+        <v>20.455860184034901</v>
       </c>
     </row>
     <row r="23" spans="2:90" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update demands to include review 1 comments
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_BASE.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_BASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccireland-my.sharepoint.com/personal/agaur_ucc_ie/Documents/TIM-2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{A01CDD26-5182-4BC8-9361-792A002E723C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{FB2A0E12-2244-4A7B-BA61-7303D5930D6F}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{A01CDD26-5182-4BC8-9361-792A002E723C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{BDB12956-2080-4EF2-BCA0-CBA5186E14EA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7912,107 +7912,107 @@
       </c>
       <c r="G37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.17991488188042462</v>
+        <v>0.18129579916441468</v>
       </c>
       <c r="H37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.6871723541686299</v>
+        <v>2.7077974559397995</v>
       </c>
       <c r="I37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.48763398226070803</v>
+        <v>0.49137676433257832</v>
       </c>
       <c r="J37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.3135901348759621</v>
+        <v>0.3159970621563124</v>
       </c>
       <c r="K37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.22335515894815736</v>
+        <v>0.22506949739662907</v>
       </c>
       <c r="L37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.10778652622510916</v>
+        <v>0.10861383008952448</v>
       </c>
       <c r="M37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.2824588239748011</v>
+        <v>0.2846268062337759</v>
       </c>
       <c r="N37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.43704621254646414</v>
+        <v>0.44040071364442734</v>
       </c>
       <c r="O37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.20559159765702764</v>
+        <v>0.20716959380543079</v>
       </c>
       <c r="P37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.23409610092244049</v>
+        <v>0.23589288031333783</v>
       </c>
       <c r="Q37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.47314719217489071</v>
+        <v>0.4767787824508965</v>
       </c>
       <c r="R37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.31213492756751032</v>
+        <v>0.3145306855610121</v>
       </c>
       <c r="S37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.30715715583422787</v>
+        <v>0.3095147074773133</v>
       </c>
       <c r="T37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.643458450750628</v>
+        <v>1.6560726389514095</v>
       </c>
       <c r="U37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.44716269403431846</v>
+        <v>0.45059484309555037</v>
       </c>
       <c r="V37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.50383886577623815</v>
+        <v>0.50770602668491038</v>
       </c>
       <c r="W37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.41246493081645397</v>
+        <v>0.4156307609359588</v>
       </c>
       <c r="X37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.38312416759737483</v>
+        <v>0.38606479585124626</v>
       </c>
       <c r="Y37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.61177286314532875</v>
+        <v>0.61646845981728682</v>
       </c>
       <c r="Z37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.1588596696128737E-2</v>
+        <v>8.2214821176152891E-2</v>
       </c>
       <c r="AA37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.34456408847334713</v>
+        <v>0.34720875299604825</v>
       </c>
       <c r="AB37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.15301315083761008</v>
+        <v>0.15418758678454786</v>
       </c>
       <c r="AC37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16686146187994025</v>
+        <v>0.16814218904566186</v>
       </c>
       <c r="AD37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1939549663563945</v>
+        <v>0.19544364679548829</v>
       </c>
       <c r="AE37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.40532554878448751</v>
+        <v>0.40843658134671468</v>
       </c>
       <c r="AF37" s="12">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.15629751581539669</v>
+        <v>0.15749716055172061</v>
       </c>
     </row>
     <row r="38" spans="4:32" x14ac:dyDescent="0.25">
@@ -8028,107 +8028,107 @@
       </c>
       <c r="G38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.24717940281716996</v>
+        <v>0.22284515413893349</v>
       </c>
       <c r="H38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.6918216593759139</v>
+        <v>3.328370233767433</v>
       </c>
       <c r="I38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.66994500548692359</v>
+        <v>0.60399044706313865</v>
       </c>
       <c r="J38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.43083163248003559</v>
+        <v>0.38841724048890991</v>
       </c>
       <c r="K38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.30686063447287587</v>
+        <v>0.27665090460170355</v>
       </c>
       <c r="L38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14808452144479622</v>
+        <v>0.13350593791734622</v>
       </c>
       <c r="M38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.38806130266052169</v>
+        <v>0.34985755213068354</v>
       </c>
       <c r="N38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.60044405827717617</v>
+        <v>0.54133170965525701</v>
       </c>
       <c r="O38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.28245583579276529</v>
+        <v>0.25464870271265072</v>
       </c>
       <c r="P38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.32161727714272298</v>
+        <v>0.28995478944346598</v>
       </c>
       <c r="Q38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.65004205980103025</v>
+        <v>0.58604690100451995</v>
       </c>
       <c r="R38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.42883236888539111</v>
+        <v>0.38661479983716018</v>
       </c>
       <c r="S38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.4219935647157021</v>
+        <v>0.3804492603466082</v>
       </c>
       <c r="T38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.2578959237033009</v>
+        <v>2.0356112176527206</v>
       </c>
       <c r="U38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.6143427743069082</v>
+        <v>0.55386212877868946</v>
       </c>
       <c r="V38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.69220838574888921</v>
+        <v>0.62406204829522471</v>
       </c>
       <c r="W38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.56667260771677863</v>
+        <v>0.51088498140907812</v>
       </c>
       <c r="X38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.52636225509396406</v>
+        <v>0.4745430911008866</v>
       </c>
       <c r="Y38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.84049551316447058</v>
+        <v>0.75775064608744125</v>
       </c>
       <c r="Z38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.11209200927271526</v>
+        <v>0.10105680651149243</v>
       </c>
       <c r="AA38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.47338577404447152</v>
+        <v>0.42678202383289654</v>
       </c>
       <c r="AB38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.21021995986052533</v>
+        <v>0.18952428407981023</v>
       </c>
       <c r="AC38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.229245719251261</v>
+        <v>0.20667700083418633</v>
       </c>
       <c r="AD38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.26646863370235813</v>
+        <v>0.24023540421980563</v>
       </c>
       <c r="AE38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.5568640350812033</v>
+        <v>0.50204204038751388</v>
       </c>
       <c r="AF38" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.2147322457001285</v>
+        <v>0.19359234566578742</v>
       </c>
     </row>
     <row r="39" spans="4:32" x14ac:dyDescent="0.25">
@@ -8144,107 +8144,107 @@
       </c>
       <c r="G39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.27465234427286017</v>
+        <v>0.24603905677094148</v>
       </c>
       <c r="H39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.1021519666624968</v>
+        <v>3.6747896810449197</v>
       </c>
       <c r="I39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.74440654922601956</v>
+        <v>0.6668542579185972</v>
       </c>
       <c r="J39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.47871673974011858</v>
+        <v>0.42884401885572321</v>
       </c>
       <c r="K39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.34096689150661796</v>
+        <v>0.30544495295865542</v>
       </c>
       <c r="L39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1645434874499693</v>
+        <v>0.14740134316775294</v>
       </c>
       <c r="M39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.4311926693023333</v>
+        <v>0.386271007162031</v>
       </c>
       <c r="N39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.66718086673474575</v>
+        <v>0.59767394879380531</v>
       </c>
       <c r="O39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.313849603040809</v>
+        <v>0.28115274422482139</v>
       </c>
       <c r="P39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.3573636723737853</v>
+        <v>0.32013351682042884</v>
       </c>
       <c r="Q39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.72229147560635665</v>
+        <v>0.64704313317394124</v>
       </c>
       <c r="R39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.47649526648292073</v>
+        <v>0.42685397873321906</v>
       </c>
       <c r="S39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.46889635825747522</v>
+        <v>0.42004672494032907</v>
       </c>
       <c r="T39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.5088514718515604</v>
+        <v>2.2474792681889455</v>
       </c>
       <c r="U39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.68262436605726895</v>
+        <v>0.61150854400403731</v>
       </c>
       <c r="V39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.76914440970588238</v>
+        <v>0.68901492752842886</v>
       </c>
       <c r="W39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.62965586278945795</v>
+        <v>0.56405830061695206</v>
       </c>
       <c r="X39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.58486518557226785</v>
+        <v>0.52393391717567761</v>
       </c>
       <c r="Y39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.93391302192031667</v>
+        <v>0.83661794195754102</v>
       </c>
       <c r="Z39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12455056032228547</v>
+        <v>0.11157488010203555</v>
       </c>
       <c r="AA39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.52600059351589779</v>
+        <v>0.47120183966474594</v>
       </c>
       <c r="AB39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.23358501610810267</v>
+        <v>0.20925012379274185</v>
       </c>
       <c r="AC39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.25472540789916959</v>
+        <v>0.22818810908397552</v>
       </c>
       <c r="AD39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.29608549129666778</v>
+        <v>0.26523929804807966</v>
       </c>
       <c r="AE39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.61875710893849889</v>
+        <v>0.55429497919121307</v>
       </c>
       <c r="AF39" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.23859882336611649</v>
+        <v>0.21374159249605457</v>
       </c>
     </row>
     <row r="40" spans="4:32" x14ac:dyDescent="0.25">
@@ -8260,107 +8260,107 @@
       </c>
       <c r="G40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.30517878666099363</v>
+        <v>0.27566537632462551</v>
       </c>
       <c r="H40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.5580887474288172</v>
+        <v>4.1172824088746074</v>
       </c>
       <c r="I40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.82714417776678117</v>
+        <v>0.7471522301191007</v>
       </c>
       <c r="J40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.53192407359558225</v>
+        <v>0.4804824461365349</v>
       </c>
       <c r="K40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.37886391436798894</v>
+        <v>0.34222451918353242</v>
       </c>
       <c r="L40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1828317977255732</v>
+        <v>0.16515039225224712</v>
       </c>
       <c r="M40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.47911790443000535</v>
+        <v>0.43278308716549024</v>
       </c>
       <c r="N40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.74133518842737034</v>
+        <v>0.66964170719877392</v>
       </c>
       <c r="O40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.34873265438023476</v>
+        <v>0.31500721088193595</v>
       </c>
       <c r="P40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.39708312783742522</v>
+        <v>0.3586817781966562</v>
       </c>
       <c r="Q40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.80257110757495254</v>
+        <v>0.72495558691202666</v>
       </c>
       <c r="R40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.52945569301420992</v>
+        <v>0.47825277916223025</v>
       </c>
       <c r="S40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.52101219839074597</v>
+        <v>0.47062584300346721</v>
       </c>
       <c r="T40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.7876996648958325</v>
+        <v>2.5181051593117307</v>
       </c>
       <c r="U40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.75849516715438692</v>
+        <v>0.68514216856852284</v>
       </c>
       <c r="V40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.85463154644670514</v>
+        <v>0.77198133411492387</v>
       </c>
       <c r="W40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.6996394395569554</v>
+        <v>0.63197829543526829</v>
       </c>
       <c r="X40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.64987046866739206</v>
+        <v>0.58702241157561752</v>
       </c>
       <c r="Y40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0377134905988405</v>
+        <v>0.9373576814853789</v>
       </c>
       <c r="Z40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.13839382648538334</v>
+        <v>0.12500995457943573</v>
       </c>
       <c r="AA40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.58446332703669712</v>
+        <v>0.52794070242663693</v>
       </c>
       <c r="AB40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.25954699926842562</v>
+        <v>0.23444657477695763</v>
       </c>
       <c r="AC40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.28303705588314848</v>
+        <v>0.25566494112355925</v>
       </c>
       <c r="AD40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.32899413701006636</v>
+        <v>0.29717757770699976</v>
       </c>
       <c r="AE40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.68752933547188644</v>
+        <v>0.62103934244818115</v>
       </c>
       <c r="AF40" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E40,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F40,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E40,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.26511806992359765</v>
+        <v>0.23947887504098309</v>
       </c>
     </row>
     <row r="41" spans="4:32" x14ac:dyDescent="0.25">
@@ -8376,107 +8376,107 @@
       </c>
       <c r="G41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.33909811342351842</v>
+        <v>0.30885909213570173</v>
       </c>
       <c r="H41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.0647009642483631</v>
+        <v>4.6130570470111945</v>
       </c>
       <c r="I41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.91907774219423721</v>
+        <v>0.83711912812002975</v>
       </c>
       <c r="J41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.59104517654820732</v>
+        <v>0.53833881526751071</v>
       </c>
       <c r="K41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.42097303030812233</v>
+        <v>0.38343282609830115</v>
       </c>
       <c r="L41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.20315277598715364</v>
+        <v>0.18503665892671434</v>
       </c>
       <c r="M41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.53236982582318593</v>
+        <v>0.4848958297766422</v>
       </c>
       <c r="N41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.82373144791823305</v>
+        <v>0.75027532474029768</v>
       </c>
       <c r="O41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.3874928086691557</v>
+        <v>0.35293819799343079</v>
       </c>
       <c r="P41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.44121723202063878</v>
+        <v>0.40187175428582139</v>
       </c>
       <c r="Q41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.89177347955448472</v>
+        <v>0.81224971883547825</v>
       </c>
       <c r="R41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.58830244594260861</v>
+        <v>0.5358406672351741</v>
       </c>
       <c r="S41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.57892049273136259</v>
+        <v>0.52729534823581425</v>
       </c>
       <c r="T41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.0975406498605595</v>
+        <v>2.8213179463327891</v>
       </c>
       <c r="U41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.84279868544278258</v>
+        <v>0.76764224433743777</v>
       </c>
       <c r="V41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.94962021522888174</v>
+        <v>0.86493798089340879</v>
       </c>
       <c r="W41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.77740139354441862</v>
+        <v>0.70807674572720203</v>
       </c>
       <c r="X41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.72210081279196892</v>
+        <v>0.65770758562383569</v>
       </c>
       <c r="Y41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1530509403561278</v>
+        <v>1.0502278028890715</v>
       </c>
       <c r="Z41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.15377571286691752</v>
+        <v>0.14006278769613009</v>
       </c>
       <c r="AA41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.64942394499895462</v>
+        <v>0.59151166616207895</v>
       </c>
       <c r="AB41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.28839454655289004</v>
+        <v>0.26267700791942911</v>
       </c>
       <c r="AC41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.31449542325344704</v>
+        <v>0.28645034301790978</v>
       </c>
       <c r="AD41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.36556043887624251</v>
+        <v>0.33296164385034366</v>
       </c>
       <c r="AE41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.76394530279335671</v>
+        <v>0.69582059976664368</v>
       </c>
       <c r="AF41" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E41,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F41,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E41,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.2945848180641813</v>
+        <v>0.26831526293579661</v>
       </c>
     </row>
     <row r="42" spans="4:32" x14ac:dyDescent="0.25">
@@ -8492,107 +8492,107 @@
       </c>
       <c r="G42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.3767874293994844</v>
+        <v>0.34604976535955428</v>
       </c>
       <c r="H42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.6276209788664602</v>
+        <v>5.1685294341507806</v>
       </c>
       <c r="I42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0212293321347361</v>
+        <v>0.93791921701516134</v>
       </c>
       <c r="J42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.65673733917954047</v>
+        <v>0.60316184775098813</v>
       </c>
       <c r="K42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.46776239577069745</v>
+        <v>0.42960315199064952</v>
       </c>
       <c r="L42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.225732344738725</v>
+        <v>0.20731749213447806</v>
       </c>
       <c r="M42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.59154047227399698</v>
+        <v>0.5432836280057084</v>
       </c>
       <c r="N42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.91528570195548664</v>
+        <v>0.84061828417008377</v>
       </c>
       <c r="O42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.43056098960623501</v>
+        <v>0.39543657192513287</v>
       </c>
       <c r="P42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.4902566545753077</v>
+        <v>0.45026236823275895</v>
       </c>
       <c r="Q42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.99089031659786231</v>
+        <v>0.91005520566927378</v>
       </c>
       <c r="R42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.65368976570888504</v>
+        <v>0.60036289003067056</v>
       </c>
       <c r="S42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.64326504822071484</v>
+        <v>0.59078860288826129</v>
       </c>
       <c r="T42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.441819145315312</v>
+        <v>3.1610415176128361</v>
       </c>
       <c r="U42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.93647218199836324</v>
+        <v>0.86007640797033158</v>
       </c>
       <c r="V42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0551664714070321</v>
+        <v>0.96908782341179667</v>
       </c>
       <c r="W42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.86380625868991667</v>
+        <v>0.79333844447032698</v>
       </c>
       <c r="X42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.80235925311489531</v>
+        <v>0.73690417888144322</v>
       </c>
       <c r="Y42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.2812076581529919</v>
+        <v>1.1766889627589938</v>
       </c>
       <c r="Z42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.17086723063785866</v>
+        <v>0.15692817874552148</v>
       </c>
       <c r="AA42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.72160465994989298</v>
+        <v>0.66273740516238988</v>
       </c>
       <c r="AB42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.32044837628682882</v>
+        <v>0.29430675434327275</v>
       </c>
       <c r="AC42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.34945025464524043</v>
+        <v>0.32094270983921375</v>
       </c>
       <c r="AD42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.40619093000466633</v>
+        <v>0.37305457945696069</v>
       </c>
       <c r="AE42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.8488545805674067</v>
+        <v>0.77960649827914863</v>
       </c>
       <c r="AF42" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E42,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F42,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E42,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.32732667020146111</v>
+        <v>0.3006239289874113</v>
       </c>
     </row>
     <row r="43" spans="4:32" x14ac:dyDescent="0.25">
@@ -8608,107 +8608,107 @@
       </c>
       <c r="G43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.41866575299274367</v>
+        <v>0.38771868193146314</v>
       </c>
       <c r="H43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.2531071655707198</v>
+        <v>5.790887959859683</v>
       </c>
       <c r="I43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1347346380368684</v>
+        <v>1.0508569546390769</v>
       </c>
       <c r="J43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.72973090706414478</v>
+        <v>0.67579042094819974</v>
       </c>
       <c r="K43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.51975220075454243</v>
+        <v>0.48133298882705872</v>
       </c>
       <c r="L43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.25082153678926639</v>
+        <v>0.23228122899664036</v>
       </c>
       <c r="M43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.65728768511462199</v>
+        <v>0.60870208059946274</v>
       </c>
       <c r="N43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0170158230156978</v>
+        <v>0.94183971720735149</v>
       </c>
       <c r="O43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.47841601618740709</v>
+        <v>0.44305230577170701</v>
       </c>
       <c r="P43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.54474660095376171</v>
+        <v>0.50447984483722008</v>
       </c>
       <c r="Q43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1010235696897956</v>
+        <v>1.0196377519873254</v>
       </c>
       <c r="R43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.72634460873692575</v>
+        <v>0.67265443212018861</v>
       </c>
       <c r="S43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.71476122814517573</v>
+        <v>0.66192727561588849</v>
       </c>
       <c r="T43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.8243627353355865</v>
+        <v>3.5416722489785744</v>
       </c>
       <c r="U43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0405570903943719</v>
+        <v>0.96364085354059725</v>
       </c>
       <c r="V43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1724437463011761</v>
+        <v>1.0857786687953852</v>
       </c>
       <c r="W43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.95981465812339428</v>
+        <v>0.88886676659351749</v>
       </c>
       <c r="X43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.89153807867588786</v>
+        <v>0.82563707751351578</v>
       </c>
       <c r="Y43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.423608451575975</v>
+        <v>1.3183776998380254</v>
       </c>
       <c r="Z43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.18985839811799671</v>
+        <v>0.17582438340306403</v>
       </c>
       <c r="AA43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.80180795522423032</v>
+        <v>0.7425396544605557</v>
       </c>
       <c r="AB43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.35606485324430737</v>
+        <v>0.32974513581576725</v>
       </c>
       <c r="AC43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.38829016729069199</v>
+        <v>0.35958840863562042</v>
       </c>
       <c r="AD43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.45133732789403713</v>
+        <v>0.41797522875146098</v>
       </c>
       <c r="AE43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.94320116443640356</v>
+        <v>0.8734813145269178</v>
       </c>
       <c r="AF43" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E43,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F43,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E43,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.36370764033427094</v>
+        <v>0.33682298088817003</v>
       </c>
     </row>
     <row r="44" spans="4:32" x14ac:dyDescent="0.25">
@@ -8724,107 +8724,107 @@
       </c>
       <c r="G44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.46519867440816737</v>
+        <v>0.43440508090643798</v>
       </c>
       <c r="H44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.948113485666763</v>
+        <v>6.4881865898008062</v>
       </c>
       <c r="I44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.2608555766655507</v>
+        <v>1.1773938726062627</v>
       </c>
       <c r="J44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.81083740003638038</v>
+        <v>0.75716442402353001</v>
       </c>
       <c r="K44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.57752045177655487</v>
+        <v>0.53929177441936482</v>
       </c>
       <c r="L44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.2786992859896244</v>
+        <v>0.2602509261938768</v>
       </c>
       <c r="M44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.73034242145293082</v>
+        <v>0.68199777027372843</v>
       </c>
       <c r="N44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1300528150131115</v>
+        <v>1.0552495343174608</v>
       </c>
       <c r="O44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.53158992574650732</v>
+        <v>0.49640159657966676</v>
       </c>
       <c r="P44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.60529287346901073</v>
+        <v>0.56522581455313703</v>
       </c>
       <c r="Q44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.2233976661585662</v>
+        <v>1.1424154697441435</v>
       </c>
       <c r="R44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.80707472902325783</v>
+        <v>0.75365082113556114</v>
       </c>
       <c r="S44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.79420390484447489</v>
+        <v>0.74163197472369236</v>
       </c>
       <c r="T44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.2494244208337317</v>
+        <v>3.9681358973916749</v>
       </c>
       <c r="U44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1562105943398513</v>
+        <v>1.0796758125290689</v>
       </c>
       <c r="V44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.3027558922568623</v>
+        <v>1.2165206177708001</v>
       </c>
       <c r="W44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0664939834337732</v>
+        <v>0.9958979477944182</v>
       </c>
       <c r="X44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.99062875198109601</v>
+        <v>0.92505457738044761</v>
       </c>
       <c r="Y44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.5818364884526053</v>
+        <v>1.4771276135324805</v>
       </c>
       <c r="Z44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.210960353213512</v>
+        <v>0.1969959381813696</v>
       </c>
       <c r="AA44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.89092550616792421</v>
+        <v>0.8319511380398108</v>
       </c>
       <c r="AB44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.39563995036264976</v>
+        <v>0.36945076179711606</v>
       </c>
       <c r="AC44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.43144697128471887</v>
+        <v>0.40288755488441136</v>
       </c>
       <c r="AD44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.50150155618501124</v>
+        <v>0.46830491158731807</v>
       </c>
       <c r="AE44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0480339704395638</v>
+        <v>0.97865988612434685</v>
       </c>
       <c r="AF44" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E44,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F44,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E44,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.40413220079779938</v>
+        <v>0.37738087196359965</v>
       </c>
     </row>
     <row r="45" spans="4:32" x14ac:dyDescent="0.25">
@@ -8840,107 +8840,107 @@
       </c>
       <c r="G45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.51690353260911526</v>
+        <v>0.48671313277260853</v>
       </c>
       <c r="H45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.7203668094698417</v>
+        <v>7.2694490924136357</v>
       </c>
       <c r="I45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.400994322517106</v>
+        <v>1.3191674900480539</v>
       </c>
       <c r="J45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.90095853558398908</v>
+        <v>0.8483369210864089</v>
       </c>
       <c r="K45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.64170939880062627</v>
+        <v>0.60422955564527769</v>
       </c>
       <c r="L45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.30967552873393511</v>
+        <v>0.29158854065538958</v>
       </c>
       <c r="M45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.81151688177873116</v>
+        <v>0.76411921937292582</v>
       </c>
       <c r="N45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.2556533890778794</v>
+        <v>1.1823153763137209</v>
       </c>
       <c r="O45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.5906738897469278</v>
+        <v>0.55617483957709746</v>
       </c>
       <c r="P45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.67256860728870715</v>
+        <v>0.63328639331536341</v>
       </c>
       <c r="Q45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.3593731242412317</v>
+        <v>1.2799772301162851</v>
       </c>
       <c r="R45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.89677765965779821</v>
+        <v>0.84440023446811752</v>
       </c>
       <c r="S45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.882476297999647</v>
+        <v>0.83093416179413448</v>
       </c>
       <c r="T45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>4.7217299092239964</v>
+        <v>4.4459513453594255</v>
       </c>
       <c r="U45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.2847184945543797</v>
+        <v>1.2096828978112597</v>
       </c>
       <c r="V45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.4475516803473705</v>
+        <v>1.3630056069376884</v>
       </c>
       <c r="W45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1850302631335401</v>
+        <v>1.1158170827132454</v>
       </c>
       <c r="X45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1007329332024371</v>
+        <v>1.0364432441789297</v>
       </c>
       <c r="Y45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.7576509002984255</v>
+        <v>1.654993092592683</v>
       </c>
       <c r="Z45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.23440770108655448</v>
+        <v>0.22071682498664011</v>
       </c>
       <c r="AA45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.98994809479121493</v>
+        <v>0.93212893335449976</v>
       </c>
       <c r="AB45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.4396136516165407</v>
+        <v>0.41393746432314377</v>
       </c>
       <c r="AC45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.47940047093706689</v>
+        <v>0.45140048450566361</v>
       </c>
       <c r="AD45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.55724132561382422</v>
+        <v>0.52469494632949409</v>
       </c>
       <c r="AE45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1645184980455237</v>
+        <v>1.0965033330193856</v>
       </c>
       <c r="AF45" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E45,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F45,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E45,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.44904977964359233</v>
+        <v>0.42282246344494845</v>
       </c>
     </row>
     <row r="46" spans="4:32" x14ac:dyDescent="0.25">
@@ -8956,107 +8956,107 @@
       </c>
       <c r="G46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.57435516625091065</v>
+        <v>0.54531975804479138</v>
       </c>
       <c r="H46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.5784528110862226</v>
+        <v>8.1447858158493265</v>
       </c>
       <c r="I46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.5567088949155781</v>
+        <v>1.4780125048108099</v>
       </c>
       <c r="J46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0010962526770586</v>
+        <v>0.95048777893453018</v>
       </c>
       <c r="K46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.71303267472853427</v>
+        <v>0.67698669483392715</v>
       </c>
       <c r="L46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.34409464932854172</v>
+        <v>0.32669961365747568</v>
       </c>
       <c r="M46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.90171353868829107</v>
+        <v>0.85612916473428158</v>
       </c>
       <c r="N46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.3952139336271721</v>
+        <v>1.3246816071537073</v>
       </c>
       <c r="O46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.65632478546478845</v>
+        <v>0.62314556260490594</v>
       </c>
       <c r="P46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.74732175325751848</v>
+        <v>0.7095423556962791</v>
       </c>
       <c r="Q46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.5104616771133752</v>
+        <v>1.4341032251454735</v>
       </c>
       <c r="R46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.99645069013748588</v>
+        <v>0.94607706377269418</v>
       </c>
       <c r="S46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.98055979283345573</v>
+        <v>0.93098949987122714</v>
       </c>
       <c r="T46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.2465301471542354</v>
+        <v>4.9813020210059182</v>
       </c>
       <c r="U46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.4275095022099455</v>
+        <v>1.3553445360874452</v>
       </c>
       <c r="V46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.6084409054550108</v>
+        <v>1.5271293041854501</v>
       </c>
       <c r="W46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.3167413469954343</v>
+        <v>1.2501760494958973</v>
       </c>
       <c r="X46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.2230747266442452</v>
+        <v>1.1612445629382055</v>
       </c>
       <c r="Y46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.9530063374810891</v>
+        <v>1.854275901036945</v>
       </c>
       <c r="Z46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.26046112211400196</v>
+        <v>0.24729401672907333</v>
       </c>
       <c r="AA46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.099976623672148</v>
+        <v>1.0443694451139989</v>
       </c>
       <c r="AB46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.48847484304450578</v>
+        <v>0.463780947525472</v>
       </c>
       <c r="AC46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.53268379845653313</v>
+        <v>0.5057550051909826</v>
       </c>
       <c r="AD46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.61917633373349845</v>
+        <v>0.58787507859049748</v>
       </c>
       <c r="AE46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.2939497862804947</v>
+        <v>1.228536671799233</v>
       </c>
       <c r="AF46" s="10">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E46,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F46,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E46,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.49895975664992409</v>
+        <v>0.47373581671860376</v>
       </c>
     </row>
     <row r="47" spans="4:32" x14ac:dyDescent="0.25">
@@ -9072,107 +9072,107 @@
       </c>
       <c r="G47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.63819230517154213</v>
+        <v>0.61098338731895729</v>
       </c>
       <c r="H47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.5319114304279697</v>
+        <v>9.1255245263757239</v>
       </c>
       <c r="I47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.7297304812493131</v>
+        <v>1.655984536351444</v>
       </c>
       <c r="J47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1123638520828778</v>
+        <v>1.0649389357555454</v>
       </c>
       <c r="K47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.79228323010999346</v>
+        <v>0.75850474492714726</v>
       </c>
       <c r="L47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.38233930911703939</v>
+        <v>0.36603851894881062</v>
       </c>
       <c r="M47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0019351712568612</v>
+        <v>0.95921831060618978</v>
       </c>
       <c r="N47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.5502860404671568</v>
+        <v>1.4841905937166016</v>
       </c>
       <c r="O47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.72927249964703711</v>
+        <v>0.69818043637041738</v>
       </c>
       <c r="P47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.83038339418000828</v>
+        <v>0.79498053304347149</v>
       </c>
       <c r="Q47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.6783430814813012</v>
+        <v>1.6067880052724084</v>
       </c>
       <c r="R47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1072019549847791</v>
+        <v>1.0599971128152945</v>
       </c>
       <c r="S47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.0895448518931483</v>
+        <v>1.0430928089405167</v>
       </c>
       <c r="T47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>5.8296597045000338</v>
+        <v>5.5811159180536754</v>
       </c>
       <c r="U47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.5861711244217456</v>
+        <v>1.5185457402314229</v>
       </c>
       <c r="V47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.7872122851874988</v>
+        <v>1.7110156406044432</v>
       </c>
       <c r="W47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.4630915589024098</v>
+        <v>1.4007135927088417</v>
       </c>
       <c r="X47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.3590142912602505</v>
+        <v>1.3010735923333812</v>
       </c>
       <c r="Y47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.1700747025007034</v>
+        <v>2.0775549653684253</v>
       </c>
       <c r="Z47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.28941027032894368</v>
+        <v>0.27707144987112264</v>
       </c>
       <c r="AA47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.2222343566236267</v>
+        <v>1.1701251821060177</v>
       </c>
       <c r="AB47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.54276674855344553</v>
+        <v>0.51962623784087003</v>
       </c>
       <c r="AC47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.59188934171786778</v>
+        <v>0.56665452088703194</v>
       </c>
       <c r="AD47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.6879951551796788</v>
+        <v>0.65866292489647515</v>
       </c>
       <c r="AE47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.4377668129511041</v>
+        <v>1.3764685509887571</v>
       </c>
       <c r="AF47" s="9">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E47,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F47,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CL$25,MATCH($E47,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.55441701580366332</v>
+        <v>0.53077980345115405</v>
       </c>
     </row>
     <row r="48" spans="4:32" x14ac:dyDescent="0.25">
@@ -16330,8 +16330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20:CL20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18492,7 +18492,6 @@
         <v>24</v>
       </c>
       <c r="H10" s="28">
-        <f>VLOOKUP(F10,'BY-Demands'!$I$5:$J$38,2,FALSE)</f>
         <v>17.770098364755199</v>
       </c>
       <c r="I10">
@@ -18502,244 +18501,244 @@
         <v>16.2067419529189</v>
       </c>
       <c r="K10">
-        <v>16.349570779521098</v>
+        <v>18.038812365039959</v>
       </c>
       <c r="L10">
-        <v>16.493227903926901</v>
+        <v>18.752348682008719</v>
       </c>
       <c r="M10">
-        <v>16.637695333555801</v>
+        <v>19.494109366820016</v>
       </c>
       <c r="N10">
-        <v>16.782954916422302</v>
+        <v>20.265210851701845</v>
       </c>
       <c r="O10">
-        <v>16.928988363644599</v>
+        <v>21.066813730045585</v>
       </c>
       <c r="P10">
-        <v>17.075777269136498</v>
+        <v>21.900124503227982</v>
       </c>
       <c r="Q10">
-        <v>17.223303130798499</v>
+        <v>21.903403629125965</v>
       </c>
       <c r="R10">
-        <v>17.371547369874801</v>
+        <v>21.906683246010498</v>
       </c>
       <c r="S10">
-        <v>17.5204913490997</v>
+        <v>21.909963353955103</v>
       </c>
       <c r="T10">
-        <v>17.6701163965215</v>
+        <v>21.913243953033305</v>
       </c>
       <c r="U10">
-        <v>17.820499435879601</v>
+        <v>21.916525043318639</v>
       </c>
       <c r="V10">
-        <v>17.9715214278974</v>
+        <v>22.110531640458859</v>
       </c>
       <c r="W10">
-        <v>18.123164107833301</v>
+        <v>22.306255597429594</v>
       </c>
       <c r="X10">
-        <v>18.275409227469801</v>
+        <v>22.503712116418974</v>
       </c>
       <c r="Y10">
-        <v>18.428238577973801</v>
+        <v>22.702916534185945</v>
       </c>
       <c r="Z10">
-        <v>18.581634006474498</v>
+        <v>22.903884323251511</v>
       </c>
       <c r="AA10">
-        <v>18.7355774375288</v>
+        <v>23.057513384534978</v>
       </c>
       <c r="AB10">
-        <v>18.8900508848699</v>
+        <v>23.212172921179643</v>
       </c>
       <c r="AC10">
-        <v>19.045036469638301</v>
+        <v>23.367869845155557</v>
       </c>
       <c r="AD10">
-        <v>19.2005164386239</v>
+        <v>23.524611114795182</v>
       </c>
       <c r="AE10">
-        <v>19.356473182002699</v>
+        <v>23.68240373510438</v>
       </c>
       <c r="AF10">
-        <v>19.512889241122199</v>
+        <v>23.806316159658131</v>
       </c>
       <c r="AG10">
-        <v>19.669747338462599</v>
+        <v>23.930876925872237</v>
       </c>
       <c r="AH10">
-        <v>19.8270303823742</v>
+        <v>24.056089426036937</v>
       </c>
       <c r="AI10">
-        <v>19.984721483951599</v>
+        <v>24.18195707019181</v>
       </c>
       <c r="AJ10">
-        <v>20.142803975179199</v>
+        <v>24.308483286218632</v>
       </c>
       <c r="AK10">
-        <v>20.301261431355801</v>
+        <v>24.436054231032401</v>
       </c>
       <c r="AL10">
-        <v>20.460077669916402</v>
+        <v>24.564294668293275</v>
       </c>
       <c r="AM10">
-        <v>20.619236784569999</v>
+        <v>24.69320811149829</v>
       </c>
       <c r="AN10">
-        <v>20.7787231433072</v>
+        <v>24.822798092583323</v>
       </c>
       <c r="AO10">
-        <v>20.938521428915699</v>
+        <v>24.953068162019846</v>
       </c>
       <c r="AP10">
-        <v>21.098616629476599</v>
+        <v>25.114582809575673</v>
       </c>
       <c r="AQ10">
-        <v>21.2589940720949</v>
+        <v>25.277142898966776</v>
       </c>
       <c r="AR10">
-        <v>21.4196394434823</v>
+        <v>25.440755197063204</v>
       </c>
       <c r="AS10">
-        <v>21.743313076624901</v>
+        <v>25.605426514535175</v>
       </c>
       <c r="AT10">
-        <v>21.9372286853426</v>
+        <v>25.771163706136587</v>
       </c>
       <c r="AU10">
-        <v>22.132818489197501</v>
+        <v>25.937973670990353</v>
       </c>
       <c r="AV10">
-        <v>22.3298325363473</v>
+        <v>26.105863352875595</v>
       </c>
       <c r="AW10">
-        <v>22.527913088200702</v>
+        <v>26.274839740516697</v>
       </c>
       <c r="AX10">
-        <v>22.726789098234899</v>
+        <v>26.444909867874209</v>
       </c>
       <c r="AY10">
-        <v>22.449961818974302</v>
+        <v>26.616080814437662</v>
       </c>
       <c r="AZ10">
-        <v>22.577839944459399</v>
+        <v>26.788359705520261</v>
       </c>
       <c r="BA10">
-        <v>22.704177660436599</v>
+        <v>26.961753712555488</v>
       </c>
       <c r="BB10">
-        <v>22.8291086485366</v>
+        <v>27.136270053395631</v>
       </c>
       <c r="BC10">
-        <v>22.952751874080501</v>
+        <v>27.311915992612235</v>
       </c>
       <c r="BD10">
-        <v>23.075225720765701</v>
+        <v>27.488698841798506</v>
       </c>
       <c r="BE10">
-        <v>23.1966331227732</v>
+        <v>27.66662595987367</v>
       </c>
       <c r="BF10">
-        <v>23.3170953034532</v>
+        <v>27.845704753389303</v>
       </c>
       <c r="BG10">
-        <v>23.436726823045898</v>
+        <v>28.025942676837641</v>
       </c>
       <c r="BH10">
-        <v>23.5556336835228</v>
+        <v>28.207347232961887</v>
       </c>
       <c r="BI10">
-        <v>23.673882340379802</v>
+        <v>28.389925973068525</v>
       </c>
       <c r="BJ10">
-        <v>23.791536313506601</v>
+        <v>28.573686497341665</v>
       </c>
       <c r="BK10">
-        <v>23.908663922296601</v>
+        <v>28.758636455159408</v>
       </c>
       <c r="BL10">
-        <v>24.0253266297875</v>
+        <v>28.944783545412268</v>
       </c>
       <c r="BM10">
-        <v>24.1415886920818</v>
+        <v>29.132135516823649</v>
       </c>
       <c r="BN10">
-        <v>24.257444094529301</v>
+        <v>29.320700168272406</v>
       </c>
       <c r="BO10">
-        <v>24.3729078967413</v>
+        <v>29.510485349117488</v>
       </c>
       <c r="BP10">
-        <v>24.4879950961245</v>
+        <v>29.701498959524677</v>
       </c>
       <c r="BQ10">
-        <v>24.602695496898299</v>
+        <v>29.893748950795452</v>
       </c>
       <c r="BR10">
-        <v>24.716980017214699</v>
+        <v>30.087243325697976</v>
       </c>
       <c r="BS10">
-        <v>24.830849160353701</v>
+        <v>30.281990138800222</v>
       </c>
       <c r="BT10">
-        <v>24.944241625869601</v>
+        <v>30.477997496805266</v>
       </c>
       <c r="BU10">
-        <v>25.057091694419</v>
+        <v>30.675273558888744</v>
       </c>
       <c r="BV10">
-        <v>25.169307778258901</v>
+        <v>30.873826537038482</v>
       </c>
       <c r="BW10">
-        <v>25.2807849910348</v>
+        <v>31.073664696396353</v>
       </c>
       <c r="BX10">
-        <v>25.391506530552999</v>
+        <v>31.274796355602309</v>
       </c>
       <c r="BY10">
-        <v>25.501439027646601</v>
+        <v>31.47722988714068</v>
       </c>
       <c r="BZ10">
-        <v>25.610473144898101</v>
+        <v>31.68097371768868</v>
       </c>
       <c r="CA10">
-        <v>25.718468018403101</v>
+        <v>31.886036328467188</v>
       </c>
       <c r="CB10">
-        <v>25.8253707036734</v>
+        <v>32.0924262555938</v>
       </c>
       <c r="CC10">
-        <v>25.931118305301901</v>
+        <v>32.300152090438154</v>
       </c>
       <c r="CD10">
-        <v>26.035736364148001</v>
+        <v>32.509222479979556</v>
       </c>
       <c r="CE10">
-        <v>26.139258382006499</v>
+        <v>32.719646127166946</v>
       </c>
       <c r="CF10">
-        <v>26.241728128696099</v>
+        <v>32.931431791281163</v>
       </c>
       <c r="CG10">
-        <v>26.343201870599099</v>
+        <v>33.144588288299566</v>
       </c>
       <c r="CH10">
-        <v>26.443710192708402</v>
+        <v>33.35912449126301</v>
       </c>
       <c r="CI10">
-        <v>26.5432829716434</v>
+        <v>33.575049330645214</v>
       </c>
       <c r="CJ10">
-        <v>26.641939430365898</v>
+        <v>33.792371794724502</v>
       </c>
       <c r="CK10">
-        <v>26.739683503976099</v>
+        <v>34.011100929957969</v>
       </c>
       <c r="CL10">
-        <v>26.8365190515382</v>
+        <v>34.231245841358039</v>
       </c>
     </row>
     <row r="11" spans="1:90" x14ac:dyDescent="0.35">
@@ -20706,90 +20705,257 @@
       <c r="F20" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="30" t="s">
         <v>44</v>
       </c>
       <c r="H20" s="28">
-        <f>VLOOKUP(F20,'BY-Demands'!$I$5:$J$38,2,FALSE)</f>
-        <v>11.625551</v>
+        <v>11.537000000000001</v>
       </c>
       <c r="I20">
-        <v>14.23064449</v>
+        <v>12.403</v>
       </c>
       <c r="J20">
         <v>11.754512350000001</v>
       </c>
       <c r="K20">
-        <v>14.843386020000001</v>
+        <v>12.787492999999998</v>
       </c>
       <c r="L20">
-        <v>15.15958067</v>
+        <v>13.183905282999998</v>
       </c>
       <c r="M20">
-        <v>15.48251091</v>
+        <v>13.592606346772996</v>
       </c>
       <c r="N20">
-        <v>15.812320229999999</v>
+        <v>14.013977143522958</v>
       </c>
       <c r="O20">
-        <v>16.149155159999999</v>
+        <v>14.448410434972168</v>
       </c>
       <c r="P20">
-        <v>16.49316537</v>
+        <v>14.737378643671612</v>
       </c>
       <c r="Q20">
-        <v>16.844503710000001</v>
+        <v>15.032126216545043</v>
       </c>
       <c r="R20">
-        <v>17.203326279999999</v>
+        <v>15.332768740875943</v>
       </c>
       <c r="S20">
-        <v>17.569792499999998</v>
+        <v>15.639424115693462</v>
       </c>
       <c r="T20">
-        <v>17.944065210000002</v>
+        <v>15.952212598007332</v>
+      </c>
+      <c r="U20">
+        <v>16.319113487761502</v>
+      </c>
+      <c r="V20">
+        <v>16.694453097980016</v>
+      </c>
+      <c r="W20">
+        <v>17.078425519233555</v>
+      </c>
+      <c r="X20">
+        <v>17.471229306175925</v>
       </c>
       <c r="Y20">
-        <v>19.9384719</v>
+        <v>17.87306758021797</v>
+      </c>
+      <c r="Z20">
+        <v>18.284148134562983</v>
+      </c>
+      <c r="AA20">
+        <v>18.704683541657932</v>
+      </c>
+      <c r="AB20">
+        <v>19.13489126311606</v>
+      </c>
+      <c r="AC20">
+        <v>19.574993762167729</v>
       </c>
       <c r="AD20">
-        <v>22.154548420000001</v>
+        <v>20.025218618697583</v>
+      </c>
+      <c r="AE20">
+        <v>20.485798646927627</v>
+      </c>
+      <c r="AF20">
+        <v>20.956972015806958</v>
+      </c>
+      <c r="AG20">
+        <v>21.438982372170514</v>
+      </c>
+      <c r="AH20">
+        <v>21.932078966730433</v>
       </c>
       <c r="AI20">
-        <v>24.616932439999999</v>
+        <v>22.436516782965231</v>
+      </c>
+      <c r="AJ20">
+        <v>22.952556668973429</v>
+      </c>
+      <c r="AK20">
+        <v>23.480465472359818</v>
+      </c>
+      <c r="AL20">
+        <v>24.020516178224089</v>
+      </c>
+      <c r="AM20">
+        <v>24.572988050323243</v>
       </c>
       <c r="AN20">
-        <v>27.353000000000002</v>
+        <v>25.138166775480673</v>
+      </c>
+      <c r="AO20">
+        <v>25.716344611316728</v>
+      </c>
+      <c r="AP20">
+        <v>26.307820537377012</v>
+      </c>
+      <c r="AQ20">
+        <v>26.912900409736679</v>
+      </c>
+      <c r="AR20">
+        <v>27.531897119160618</v>
       </c>
       <c r="AS20">
-        <v>30.39316985</v>
+        <v>28.165130752901309</v>
+      </c>
+      <c r="AT20">
+        <v>28.812928760218039</v>
+      </c>
+      <c r="AU20">
+        <v>29.475626121703051</v>
+      </c>
+      <c r="AV20">
+        <v>30.15356552250222</v>
+      </c>
+      <c r="AW20">
+        <v>30.847097529519768</v>
       </c>
       <c r="AX20">
-        <v>33.771241680000003</v>
+        <v>31.55658077269872</v>
+      </c>
+      <c r="AY20">
+        <v>32.282382130470786</v>
+      </c>
+      <c r="AZ20">
+        <v>33.024876919471609</v>
+      </c>
+      <c r="BA20">
+        <v>33.784449088619454</v>
+      </c>
+      <c r="BB20">
+        <v>34.561491417657699</v>
       </c>
       <c r="BC20">
-        <v>37.52477185</v>
+        <v>35.356405720263822</v>
+      </c>
+      <c r="BD20">
+        <v>36.169603051829888</v>
+      </c>
+      <c r="BE20">
+        <v>37.001503922021968</v>
+      </c>
+      <c r="BF20">
+        <v>37.85253851222847</v>
+      </c>
+      <c r="BG20">
+        <v>38.723146898009716</v>
       </c>
       <c r="BH20">
-        <v>41.695490970000002</v>
+        <v>39.613779276663941</v>
+      </c>
+      <c r="BI20">
+        <v>40.524896200027207</v>
+      </c>
+      <c r="BJ20">
+        <v>41.456968812627828</v>
+      </c>
+      <c r="BK20">
+        <v>42.410479095318259</v>
+      </c>
+      <c r="BL20">
+        <v>43.385920114510576</v>
       </c>
       <c r="BM20">
-        <v>46.32976781</v>
+        <v>44.383796277144313</v>
+      </c>
+      <c r="BN20">
+        <v>45.404623591518629</v>
+      </c>
+      <c r="BO20">
+        <v>46.448929934123555</v>
+      </c>
+      <c r="BP20">
+        <v>47.517255322608392</v>
+      </c>
+      <c r="BQ20">
+        <v>48.610152195028377</v>
       </c>
       <c r="BR20">
-        <v>51.479124859999999</v>
+        <v>49.728185695514021</v>
+      </c>
+      <c r="BS20">
+        <v>50.871933966510845</v>
+      </c>
+      <c r="BT20">
+        <v>52.041988447740586</v>
+      </c>
+      <c r="BU20">
+        <v>53.238954182038611</v>
+      </c>
+      <c r="BV20">
+        <v>54.463450128225503</v>
       </c>
       <c r="BW20">
-        <v>57.200811090000002</v>
+        <v>55.716109481174684</v>
+      </c>
+      <c r="BX20">
+        <v>56.997579999241694</v>
+      </c>
+      <c r="BY20">
+        <v>58.308524339224249</v>
+      </c>
+      <c r="BZ20">
+        <v>59.649620399026404</v>
+      </c>
+      <c r="CA20">
+        <v>61.021561668204008</v>
       </c>
       <c r="CB20">
-        <v>63.558438449999997</v>
+        <v>62.425057586572692</v>
+      </c>
+      <c r="CC20">
+        <v>63.860833911063864</v>
+      </c>
+      <c r="CD20">
+        <v>65.329633091018323</v>
+      </c>
+      <c r="CE20">
+        <v>66.832214652111745</v>
+      </c>
+      <c r="CF20">
+        <v>68.369355589110299</v>
       </c>
       <c r="CG20">
-        <v>70.622689109999996</v>
+        <v>69.941850767659844</v>
+      </c>
+      <c r="CH20">
+        <v>71.550513335316012</v>
+      </c>
+      <c r="CI20">
+        <v>73.196175142028267</v>
+      </c>
+      <c r="CJ20">
+        <v>74.879687170294915</v>
+      </c>
+      <c r="CK20">
+        <v>76.601919975211686</v>
       </c>
       <c r="CL20">
-        <v>78.472101249999994</v>
+        <v>78.363764134641542</v>
       </c>
     </row>
     <row r="21" spans="2:90" x14ac:dyDescent="0.35">
@@ -22610,244 +22776,244 @@
         <v>29.618106901468909</v>
       </c>
       <c r="K29">
-        <v>29.724222483976618</v>
+        <v>30.592051000616877</v>
       </c>
       <c r="L29">
-        <v>30.007740851282321</v>
+        <v>31.598021694557708</v>
       </c>
       <c r="M29">
-        <v>30.28501712549933</v>
+        <v>32.637072126664755</v>
       </c>
       <c r="N29">
-        <v>30.55681892341358</v>
+        <v>33.710290071247677</v>
       </c>
       <c r="O29">
-        <v>30.823705593690793</v>
+        <v>34.818799072335445</v>
       </c>
       <c r="P29">
-        <v>31.086450703634611</v>
+        <v>35.963759619906362</v>
       </c>
       <c r="Q29">
-        <v>31.345095906869076</v>
+        <v>36.712499803959538</v>
       </c>
       <c r="R29">
-        <v>31.60114073385974</v>
+        <v>37.47682823209901</v>
       </c>
       <c r="S29">
-        <v>31.856221576979692</v>
+        <v>38.25706944060434</v>
       </c>
       <c r="T29">
-        <v>32.110064712413809</v>
+        <v>39.053554722372212</v>
       </c>
       <c r="U29">
-        <v>32.363562717820137</v>
+        <v>39.866622267584432</v>
       </c>
       <c r="V29">
-        <v>32.616435918865832</v>
+        <v>40.357314057686089</v>
       </c>
       <c r="W29">
-        <v>32.869297218876078</v>
+        <v>40.854045447311805</v>
       </c>
       <c r="X29">
-        <v>33.122473896325509</v>
+        <v>41.356890773883045</v>
       </c>
       <c r="Y29">
-        <v>33.375382800477524</v>
+        <v>41.865925289791257</v>
       </c>
       <c r="Z29">
-        <v>33.627756158034707</v>
+        <v>42.381225173659615</v>
       </c>
       <c r="AA29">
-        <v>33.879284542075581</v>
+        <v>42.776493751275368</v>
       </c>
       <c r="AB29">
-        <v>34.129783486550842</v>
+        <v>43.175448802036009</v>
       </c>
       <c r="AC29">
-        <v>34.378586533475783</v>
+        <v>43.578124707840381</v>
       </c>
       <c r="AD29">
-        <v>34.625318800234034</v>
+        <v>43.984556171250162</v>
       </c>
       <c r="AE29">
-        <v>34.869813672329414</v>
+        <v>44.394778218480539</v>
       </c>
       <c r="AF29">
-        <v>35.111595108344304</v>
+        <v>44.717758131431516</v>
       </c>
       <c r="AG29">
-        <v>35.350038303918048</v>
+        <v>45.043087780733387</v>
       </c>
       <c r="AH29">
-        <v>35.583857947223052</v>
+        <v>45.370784261136308</v>
       </c>
       <c r="AI29">
-        <v>35.812697007196086</v>
+        <v>45.700864791757795</v>
       </c>
       <c r="AJ29">
-        <v>36.036376968305539</v>
+        <v>46.033346716987502</v>
       </c>
       <c r="AK29">
-        <v>36.254332531367986</v>
+        <v>46.369255228359584</v>
       </c>
       <c r="AL29">
-        <v>36.466194764284744</v>
+        <v>46.707614887346587</v>
       </c>
       <c r="AM29">
-        <v>36.670993732667412</v>
+        <v>47.048443580142006</v>
       </c>
       <c r="AN29">
-        <v>36.868669931338765</v>
+        <v>47.391759323456121</v>
       </c>
       <c r="AO29">
-        <v>37.059265013922854</v>
+        <v>47.737580265468395</v>
       </c>
       <c r="AP29">
-        <v>37.248845640344939</v>
+        <v>48.167218487857603</v>
       </c>
       <c r="AQ29">
-        <v>37.432908554002502</v>
+        <v>48.600723454248318</v>
       </c>
       <c r="AR29">
-        <v>37.611981976403072</v>
+        <v>49.038129965336545</v>
       </c>
       <c r="AS29">
-        <v>37.786791138794861</v>
+        <v>49.47947313502457</v>
       </c>
       <c r="AT29">
-        <v>37.957710322791961</v>
+        <v>49.924788393239787</v>
       </c>
       <c r="AU29">
-        <v>38.124982970024824</v>
+        <v>50.374111488778937</v>
       </c>
       <c r="AV29">
-        <v>38.289389074356244</v>
+        <v>50.827478492177939</v>
       </c>
       <c r="AW29">
-        <v>38.451637497160185</v>
+        <v>51.284925798607532</v>
       </c>
       <c r="AX29">
-        <v>38.612502948239687</v>
+        <v>51.746490130794996</v>
       </c>
       <c r="AY29">
-        <v>38.772402624342654</v>
+        <v>52.212208541972146</v>
       </c>
       <c r="AZ29">
-        <v>38.931986316053639</v>
+        <v>52.682118418849889</v>
       </c>
       <c r="BA29">
-        <v>39.091760799214285</v>
+        <v>53.15625748461953</v>
       </c>
       <c r="BB29">
-        <v>39.252304368938745</v>
+        <v>53.634663801981098</v>
       </c>
       <c r="BC29">
-        <v>39.414123747514004</v>
+        <v>54.117375776198919</v>
       </c>
       <c r="BD29">
-        <v>39.57773749875733</v>
+        <v>54.604432158184707</v>
       </c>
       <c r="BE29">
-        <v>39.743586573883356</v>
+        <v>55.095872047608367</v>
       </c>
       <c r="BF29">
-        <v>39.912236944484022</v>
+        <v>55.59173489603684</v>
       </c>
       <c r="BG29">
-        <v>40.084230530158642</v>
+        <v>56.092060510101163</v>
       </c>
       <c r="BH29">
-        <v>40.260073255824842</v>
+        <v>56.59688905469207</v>
       </c>
       <c r="BI29">
-        <v>40.440044426883368</v>
+        <v>57.106261056184294</v>
       </c>
       <c r="BJ29">
-        <v>40.624417225652259</v>
+        <v>57.620217405689949</v>
       </c>
       <c r="BK29">
-        <v>40.813506375013745</v>
+        <v>58.138799362341153</v>
       </c>
       <c r="BL29">
-        <v>41.007596613191261</v>
+        <v>58.662048556602215</v>
       </c>
       <c r="BM29">
-        <v>41.207002258431835</v>
+        <v>59.190006993611632</v>
       </c>
       <c r="BN29">
-        <v>41.411609013191089</v>
+        <v>59.722717056554131</v>
       </c>
       <c r="BO29">
-        <v>41.621439477535333</v>
+        <v>60.260221510063111</v>
       </c>
       <c r="BP29">
-        <v>41.836522202048585</v>
+        <v>60.802563503653673</v>
       </c>
       <c r="BQ29">
-        <v>42.056731125012938</v>
+        <v>61.349786575186549</v>
       </c>
       <c r="BR29">
-        <v>42.281821400475749</v>
+        <v>61.901934654363224</v>
       </c>
       <c r="BS29">
-        <v>42.511738533595747</v>
+        <v>62.45905206625249</v>
       </c>
       <c r="BT29">
-        <v>42.746029922044585</v>
+        <v>63.021183534848753</v>
       </c>
       <c r="BU29">
-        <v>42.984207575765055</v>
+        <v>63.588374186662385</v>
       </c>
       <c r="BV29">
-        <v>43.225605524714936</v>
+        <v>64.160669554342334</v>
       </c>
       <c r="BW29">
-        <v>43.469457068488012</v>
+        <v>64.73811558033141</v>
       </c>
       <c r="BX29">
-        <v>43.715565976861427</v>
+        <v>65.320758620554386</v>
       </c>
       <c r="BY29">
-        <v>43.963623221598397</v>
+        <v>65.908645448139367</v>
       </c>
       <c r="BZ29">
-        <v>44.212803096959028</v>
+        <v>66.501823257172617</v>
       </c>
       <c r="CA29">
-        <v>44.462048303053699</v>
+        <v>67.100339666487159</v>
       </c>
       <c r="CB29">
-        <v>44.710877710772145</v>
+        <v>67.704242723485535</v>
       </c>
       <c r="CC29">
-        <v>44.958732881877857</v>
+        <v>68.313580907996894</v>
       </c>
       <c r="CD29">
-        <v>45.205655327182448</v>
+        <v>68.928403136168853</v>
       </c>
       <c r="CE29">
-        <v>45.451745991268531</v>
+        <v>69.548758764394364</v>
       </c>
       <c r="CF29">
-        <v>45.697183068339761</v>
+        <v>70.174697593273905</v>
       </c>
       <c r="CG29">
-        <v>45.942239859724516</v>
+        <v>70.806269871613367</v>
       </c>
       <c r="CH29">
-        <v>46.187017363560059</v>
+        <v>71.443526300457876</v>
       </c>
       <c r="CI29">
-        <v>46.431616595835223</v>
+        <v>72.086518037161994</v>
       </c>
       <c r="CJ29">
-        <v>46.676067255583945</v>
+        <v>72.735296699496445</v>
       </c>
       <c r="CK29">
-        <v>46.920292087234657</v>
+        <v>73.38991436979191</v>
       </c>
       <c r="CL29">
-        <v>47.164213823314761</v>
+        <v>74.050423599120023</v>
       </c>
     </row>
     <row r="30" spans="2:90" x14ac:dyDescent="0.35">
@@ -22874,244 +23040,244 @@
         <v>59.593058464401295</v>
       </c>
       <c r="K30">
-        <v>59.806568130410788</v>
+        <v>61.552680928952022</v>
       </c>
       <c r="L30">
-        <v>60.377020748965627</v>
+        <v>63.576742445676345</v>
       </c>
       <c r="M30">
-        <v>60.934913975402267</v>
+        <v>65.667361989795339</v>
       </c>
       <c r="N30">
-        <v>61.481792291687562</v>
+        <v>67.826728215642902</v>
       </c>
       <c r="O30">
-        <v>62.018781134293519</v>
+        <v>70.057101747952018</v>
       </c>
       <c r="P30">
-        <v>62.547436957915416</v>
+        <v>72.360817548486267</v>
       </c>
       <c r="Q30">
-        <v>63.06784357165224</v>
+        <v>73.867318882665543</v>
       </c>
       <c r="R30">
-        <v>63.583018103067182</v>
+        <v>75.405184515187131</v>
       </c>
       <c r="S30">
-        <v>64.096253052477209</v>
+        <v>76.975067428685819</v>
       </c>
       <c r="T30">
-        <v>64.606997674374767</v>
+        <v>78.577634200435639</v>
       </c>
       <c r="U30">
-        <v>65.117047878023641</v>
+        <v>80.21356528538071</v>
       </c>
       <c r="V30">
-        <v>65.625840945187875</v>
+        <v>81.200860814862352</v>
       </c>
       <c r="W30">
-        <v>66.134610066895249</v>
+        <v>82.200308309651447</v>
       </c>
       <c r="X30">
-        <v>66.644013743209157</v>
+        <v>83.212057340222501</v>
       </c>
       <c r="Y30">
-        <v>67.152878646743929</v>
+        <v>84.236259318013722</v>
       </c>
       <c r="Z30">
-        <v>67.660666004720426</v>
+        <v>85.273067518086194</v>
       </c>
       <c r="AA30">
-        <v>68.166753235260515</v>
+        <v>86.068366945337161</v>
       </c>
       <c r="AB30">
-        <v>68.670769183783008</v>
+        <v>86.871083734217009</v>
       </c>
       <c r="AC30">
-        <v>69.171372904704285</v>
+        <v>87.681287062763161</v>
       </c>
       <c r="AD30">
-        <v>69.667810116133538</v>
+        <v>88.499046754202112</v>
       </c>
       <c r="AE30">
-        <v>70.159745581674841</v>
+        <v>89.324433282966837</v>
       </c>
       <c r="AF30">
-        <v>70.646221483054191</v>
+        <v>89.974284433121213</v>
       </c>
       <c r="AG30">
-        <v>71.125980683786906</v>
+        <v>90.628863366053892</v>
       </c>
       <c r="AH30">
-        <v>71.596437074533128</v>
+        <v>91.288204477226031</v>
       </c>
       <c r="AI30">
-        <v>72.056872291587311</v>
+        <v>91.952342412331916</v>
       </c>
       <c r="AJ30">
-        <v>72.506927153096697</v>
+        <v>92.621312069119398</v>
       </c>
       <c r="AK30">
-        <v>72.945464249860876</v>
+        <v>93.297176182362023</v>
       </c>
       <c r="AL30">
-        <v>73.3717412727175</v>
+        <v>93.977972122733462</v>
       </c>
       <c r="AM30">
-        <v>73.783806666933216</v>
+        <v>94.663735878117009</v>
       </c>
       <c r="AN30">
-        <v>74.181540705223782</v>
+        <v>95.354503699002038</v>
       </c>
       <c r="AO30">
-        <v>74.565027196688149</v>
+        <v>96.05031210040022</v>
       </c>
       <c r="AP30">
-        <v>74.946472553465114</v>
+        <v>96.914764909303813</v>
       </c>
       <c r="AQ30">
-        <v>75.316816006246</v>
+        <v>97.786997793487544</v>
       </c>
       <c r="AR30">
-        <v>75.677120362160409</v>
+        <v>98.667080773628925</v>
       </c>
       <c r="AS30">
-        <v>76.028844821430624</v>
+        <v>99.555084500591576</v>
       </c>
       <c r="AT30">
-        <v>76.3727424567019</v>
+        <v>100.45108026109689</v>
       </c>
       <c r="AU30">
-        <v>76.709303084266807</v>
+        <v>101.35513998344675</v>
       </c>
       <c r="AV30">
-        <v>77.040096089367381</v>
+        <v>102.26733624329776</v>
       </c>
       <c r="AW30">
-        <v>77.366547735250009</v>
+        <v>103.18774226948743</v>
       </c>
       <c r="AX30">
-        <v>77.690216775373827</v>
+        <v>104.11643194991281</v>
       </c>
       <c r="AY30">
-        <v>78.011942629701494</v>
+        <v>105.05347983746201</v>
       </c>
       <c r="AZ30">
-        <v>78.3330327082043</v>
+        <v>105.99896115599915</v>
       </c>
       <c r="BA30">
-        <v>78.654506668298623</v>
+        <v>106.95295180640314</v>
       </c>
       <c r="BB30">
-        <v>78.977528067623737</v>
+        <v>107.91552837266076</v>
       </c>
       <c r="BC30">
-        <v>79.303116455841433</v>
+        <v>108.88676812801469</v>
       </c>
       <c r="BD30">
-        <v>79.632315208343059</v>
+        <v>109.86674904116681</v>
       </c>
       <c r="BE30">
-        <v>79.966011540223136</v>
+        <v>110.85554978253731</v>
       </c>
       <c r="BF30">
-        <v>80.305344213600378</v>
+        <v>111.85324973058013</v>
       </c>
       <c r="BG30">
-        <v>80.651403596825219</v>
+        <v>112.85992897815534</v>
       </c>
       <c r="BH30">
-        <v>81.005207635213836</v>
+        <v>113.87566833895872</v>
       </c>
       <c r="BI30">
-        <v>81.367318304693043</v>
+        <v>114.90054935400933</v>
       </c>
       <c r="BJ30">
-        <v>81.73828526125213</v>
+        <v>115.9346542981954</v>
       </c>
       <c r="BK30">
-        <v>82.118741742497534</v>
+        <v>116.97806618687915</v>
       </c>
       <c r="BL30">
-        <v>82.509260655457112</v>
+        <v>118.03086878256104</v>
       </c>
       <c r="BM30">
-        <v>82.910474423591765</v>
+        <v>119.09314660160408</v>
       </c>
       <c r="BN30">
-        <v>83.322153074733876</v>
+        <v>120.1649849210185</v>
       </c>
       <c r="BO30">
-        <v>83.74434208130603</v>
+        <v>121.24646978530765</v>
       </c>
       <c r="BP30">
-        <v>84.177098888459199</v>
+        <v>122.33768801337541</v>
       </c>
       <c r="BQ30">
-        <v>84.62016985394169</v>
+        <v>123.43872720549578</v>
       </c>
       <c r="BR30">
-        <v>85.073062335896992</v>
+        <v>124.54967575034523</v>
       </c>
       <c r="BS30">
-        <v>85.53566668807818</v>
+        <v>125.67062283209833</v>
       </c>
       <c r="BT30">
-        <v>86.007072252788504</v>
+        <v>126.80165843758721</v>
       </c>
       <c r="BU30">
-        <v>86.486297170515229</v>
+        <v>127.94287336352548</v>
       </c>
       <c r="BV30">
-        <v>86.972001477438482</v>
+        <v>129.0943592237972</v>
       </c>
       <c r="BW30">
-        <v>87.462642535391538</v>
+        <v>130.25620845681135</v>
       </c>
       <c r="BX30">
-        <v>87.957825519709132</v>
+        <v>131.42851433292265</v>
       </c>
       <c r="BY30">
-        <v>88.456928650685938</v>
+        <v>132.61137096191894</v>
       </c>
       <c r="BZ30">
-        <v>88.95829056858021</v>
+        <v>133.80487330057619</v>
       </c>
       <c r="CA30">
-        <v>89.459783935059846</v>
+        <v>135.00911716028136</v>
       </c>
       <c r="CB30">
-        <v>89.960440695168046</v>
+        <v>136.22419921472388</v>
       </c>
       <c r="CC30">
-        <v>90.459137244260262</v>
+        <v>137.45021700765639</v>
       </c>
       <c r="CD30">
-        <v>90.95595710408999</v>
+        <v>138.68726896072528</v>
       </c>
       <c r="CE30">
-        <v>91.451103380022232</v>
+        <v>139.93545438137178</v>
       </c>
       <c r="CF30">
-        <v>91.944934607382407</v>
+        <v>141.19487347080411</v>
       </c>
       <c r="CG30">
-        <v>92.438000681614383</v>
+        <v>142.46562733204132</v>
       </c>
       <c r="CH30">
-        <v>92.930504815837708</v>
+        <v>143.74781797802967</v>
       </c>
       <c r="CI30">
-        <v>93.422650259090148</v>
+        <v>145.04154833983193</v>
       </c>
       <c r="CJ30">
-        <v>93.914496767259266</v>
+        <v>146.3469222748904</v>
       </c>
       <c r="CK30">
-        <v>94.405888898411902</v>
+        <v>147.66404457536441</v>
       </c>
       <c r="CL30">
-        <v>94.896671186669465</v>
+        <v>148.99302097654268</v>
       </c>
     </row>
     <row r="31" spans="2:90" x14ac:dyDescent="0.35">

</xml_diff>